<commit_message>
updated excel and xml files.
</commit_message>
<xml_diff>
--- a/DividendLiberty/401k.xlsx
+++ b/DividendLiberty/401k.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steve Yi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steve Yi\Documents\GitHub\DividendLibertyCommercial\DividendLiberty\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Initial Buys" sheetId="3" r:id="rId1"/>
@@ -565,7 +565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -1198,8 +1198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1692,11 +1692,11 @@
         <v>31</v>
       </c>
       <c r="D8" s="8">
-        <v>8</v>
+        <v>8.0619999999999994</v>
       </c>
       <c r="E8" s="22">
         <f t="shared" si="0"/>
-        <v>118.5</v>
+        <v>118.47184321508311</v>
       </c>
       <c r="F8" s="9">
         <f>'Initial Buys'!T40</f>
@@ -1727,7 +1727,7 @@
         <v>0</v>
       </c>
       <c r="O8" s="26">
-        <v>0</v>
+        <v>7.12</v>
       </c>
       <c r="P8" s="23">
         <v>0</v>
@@ -1740,11 +1740,11 @@
       </c>
       <c r="S8" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7.12</v>
       </c>
       <c r="T8" s="16">
         <f t="shared" si="2"/>
-        <v>948</v>
+        <v>955.12</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -1986,7 +1986,7 @@
       </c>
       <c r="O12" s="27">
         <f t="shared" si="3"/>
-        <v>24.2</v>
+        <v>31.32</v>
       </c>
       <c r="P12" s="20">
         <f t="shared" si="3"/>
@@ -2002,11 +2002,11 @@
       </c>
       <c r="S12" s="20">
         <f>SUM(S2:S11)</f>
-        <v>33.36</v>
+        <v>40.479999999999997</v>
       </c>
       <c r="T12" s="25">
         <f>SUM(T2:T11)</f>
-        <v>9964.0700000000015</v>
+        <v>9971.19</v>
       </c>
     </row>
   </sheetData>
@@ -2572,7 +2572,7 @@
       </c>
       <c r="E8" s="22">
         <f t="shared" si="0"/>
-        <v>118.5</v>
+        <v>119.39</v>
       </c>
       <c r="F8" s="9">
         <f>'Initial Buys'!T40</f>
@@ -2580,7 +2580,7 @@
       </c>
       <c r="G8" s="18">
         <f>'2016'!S8</f>
-        <v>0</v>
+        <v>7.12</v>
       </c>
       <c r="H8" s="26">
         <v>0</v>
@@ -2624,11 +2624,11 @@
       </c>
       <c r="U8" s="18">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7.12</v>
       </c>
       <c r="V8" s="16">
         <f t="shared" si="3"/>
-        <v>948</v>
+        <v>955.12</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -2862,7 +2862,7 @@
       <c r="F12" s="13"/>
       <c r="G12" s="20">
         <f>SUM(G2:G11)</f>
-        <v>33.36</v>
+        <v>40.479999999999997</v>
       </c>
       <c r="H12" s="27">
         <f t="shared" ref="H12:S12" si="4">SUM(H2:H11)</f>
@@ -2918,11 +2918,11 @@
       </c>
       <c r="U12" s="20">
         <f>SUM(U2:U11)</f>
-        <v>33.36</v>
+        <v>40.479999999999997</v>
       </c>
       <c r="V12" s="25">
         <f>SUM(V2:V11)</f>
-        <v>9964.0700000000015</v>
+        <v>9971.19</v>
       </c>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated suzie, 401k, and total dividend excel sheets.
</commit_message>
<xml_diff>
--- a/DividendLiberty/401k.xlsx
+++ b/DividendLiberty/401k.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steve Yi\Documents\GitHub\DividendLibertyCommercial\DividendLiberty\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\Documents\GitHub\DividendLibertyCommercial\DividendLiberty\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="2016" sheetId="2" r:id="rId2"/>
     <sheet name="2017" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
@@ -376,6 +376,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -411,6 +428,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1199,7 +1233,7 @@
   <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1428,11 +1462,11 @@
         <v>13</v>
       </c>
       <c r="D4" s="8">
-        <v>20.181000000000001</v>
+        <v>20.352</v>
       </c>
       <c r="E4" s="22">
         <f t="shared" si="0"/>
-        <v>50.012387889599125</v>
+        <v>50.068297955974842</v>
       </c>
       <c r="F4" s="9">
         <f>'Initial Buys'!H40</f>
@@ -1472,15 +1506,15 @@
         <v>0</v>
       </c>
       <c r="R4" s="23">
-        <v>0</v>
+        <v>9.69</v>
       </c>
       <c r="S4" s="18">
         <f t="shared" si="1"/>
-        <v>9.5</v>
+        <v>19.189999999999998</v>
       </c>
       <c r="T4" s="16">
         <f t="shared" si="2"/>
-        <v>1009.3</v>
+        <v>1018.99</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -1626,11 +1660,11 @@
         <v>7</v>
       </c>
       <c r="D7" s="6">
-        <v>10</v>
+        <v>10.07</v>
       </c>
       <c r="E7" s="24">
         <f t="shared" si="0"/>
-        <v>87.86</v>
+        <v>87.841112214498509</v>
       </c>
       <c r="F7" s="7">
         <f>'Initial Buys'!Q40</f>
@@ -1670,15 +1704,15 @@
         <v>0</v>
       </c>
       <c r="R7" s="23">
-        <v>0</v>
+        <v>5.96</v>
       </c>
       <c r="S7" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5.96</v>
       </c>
       <c r="T7" s="17">
         <f t="shared" si="2"/>
-        <v>878.6</v>
+        <v>884.56000000000006</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -1692,11 +1726,11 @@
         <v>31</v>
       </c>
       <c r="D8" s="8">
-        <v>8.0619999999999994</v>
+        <v>8.1240000000000006</v>
       </c>
       <c r="E8" s="22">
         <f t="shared" si="0"/>
-        <v>118.47184321508311</v>
+        <v>118.49581486952239</v>
       </c>
       <c r="F8" s="9">
         <f>'Initial Buys'!T40</f>
@@ -1736,15 +1770,15 @@
         <v>0</v>
       </c>
       <c r="R8" s="23">
-        <v>0</v>
+        <v>7.54</v>
       </c>
       <c r="S8" s="18">
         <f t="shared" si="1"/>
-        <v>7.12</v>
+        <v>14.66</v>
       </c>
       <c r="T8" s="16">
         <f t="shared" si="2"/>
-        <v>955.12</v>
+        <v>962.66</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -1998,15 +2032,15 @@
       </c>
       <c r="R12" s="20">
         <f t="shared" si="3"/>
-        <v>17.100000000000001</v>
+        <v>40.29</v>
       </c>
       <c r="S12" s="20">
         <f>SUM(S2:S11)</f>
-        <v>66.78</v>
+        <v>89.969999999999985</v>
       </c>
       <c r="T12" s="25">
         <f>SUM(T2:T11)</f>
-        <v>9997.49</v>
+        <v>10020.68</v>
       </c>
     </row>
   </sheetData>
@@ -2276,7 +2310,7 @@
       </c>
       <c r="E4" s="22">
         <f t="shared" si="0"/>
-        <v>50.012387889599125</v>
+        <v>50.492542490461325</v>
       </c>
       <c r="F4" s="9">
         <f>'Initial Buys'!H40</f>
@@ -2284,7 +2318,7 @@
       </c>
       <c r="G4" s="18">
         <f>'2016'!S4</f>
-        <v>9.5</v>
+        <v>19.189999999999998</v>
       </c>
       <c r="H4" s="26">
         <v>0</v>
@@ -2328,11 +2362,11 @@
       </c>
       <c r="U4" s="18">
         <f t="shared" si="2"/>
-        <v>9.5</v>
+        <v>19.189999999999998</v>
       </c>
       <c r="V4" s="16">
         <f t="shared" si="3"/>
-        <v>1009.3</v>
+        <v>1018.99</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -2498,7 +2532,7 @@
       </c>
       <c r="E7" s="24">
         <f t="shared" si="0"/>
-        <v>87.86</v>
+        <v>88.456000000000003</v>
       </c>
       <c r="F7" s="7">
         <f>'Initial Buys'!Q40</f>
@@ -2506,7 +2540,7 @@
       </c>
       <c r="G7" s="19">
         <f>'2016'!S7</f>
-        <v>0</v>
+        <v>5.96</v>
       </c>
       <c r="H7" s="26">
         <v>0</v>
@@ -2550,11 +2584,11 @@
       </c>
       <c r="U7" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5.96</v>
       </c>
       <c r="V7" s="17">
         <f t="shared" si="3"/>
-        <v>878.6</v>
+        <v>884.56000000000006</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -2572,7 +2606,7 @@
       </c>
       <c r="E8" s="22">
         <f t="shared" si="0"/>
-        <v>119.39</v>
+        <v>120.3325</v>
       </c>
       <c r="F8" s="9">
         <f>'Initial Buys'!T40</f>
@@ -2580,7 +2614,7 @@
       </c>
       <c r="G8" s="18">
         <f>'2016'!S8</f>
-        <v>7.12</v>
+        <v>14.66</v>
       </c>
       <c r="H8" s="26">
         <v>0</v>
@@ -2624,11 +2658,11 @@
       </c>
       <c r="U8" s="18">
         <f t="shared" si="2"/>
-        <v>7.12</v>
+        <v>14.66</v>
       </c>
       <c r="V8" s="16">
         <f t="shared" si="3"/>
-        <v>955.12</v>
+        <v>962.66</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -2862,7 +2896,7 @@
       <c r="F12" s="13"/>
       <c r="G12" s="20">
         <f>SUM(G2:G11)</f>
-        <v>66.78</v>
+        <v>89.969999999999985</v>
       </c>
       <c r="H12" s="27">
         <f t="shared" ref="H12:S12" si="4">SUM(H2:H11)</f>
@@ -2918,11 +2952,11 @@
       </c>
       <c r="U12" s="20">
         <f>SUM(U2:U11)</f>
-        <v>66.78</v>
+        <v>89.969999999999985</v>
       </c>
       <c r="V12" s="25">
         <f>SUM(V2:V11)</f>
-        <v>9997.49</v>
+        <v>10020.68</v>
       </c>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated all excel files.
</commit_message>
<xml_diff>
--- a/DividendLiberty/401k.xlsx
+++ b/DividendLiberty/401k.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="53">
   <si>
     <t>Symbols</t>
   </si>
@@ -127,10 +127,64 @@
     <t>Walmart</t>
   </si>
   <si>
-    <t>Prev Year Total Dividends</t>
-  </si>
-  <si>
-    <t>2017 Dividends</t>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Telecommunications</t>
+  </si>
+  <si>
+    <t>AT&amp;T Inc.</t>
+  </si>
+  <si>
+    <t>Exxon Mobil</t>
+  </si>
+  <si>
+    <t>XOM</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>Year Dividends</t>
+  </si>
+  <si>
+    <t>All Time Dividends</t>
+  </si>
+  <si>
+    <t>Prev All Time Dividends</t>
   </si>
 </sst>
 </file>
@@ -246,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -285,6 +339,9 @@
     <xf numFmtId="4" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF40"/>
+  <dimension ref="A1:AF83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,6 +693,7 @@
     <col min="27" max="27" width="6.5703125" customWidth="1"/>
     <col min="28" max="28" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="7.140625" customWidth="1"/>
+    <col min="31" max="31" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="6.42578125" customWidth="1"/>
   </cols>
@@ -709,7 +767,12 @@
       <c r="AC1" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="AF1" s="2"/>
+      <c r="AE1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF1" s="25" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
@@ -772,7 +835,12 @@
       <c r="AC2" s="19">
         <v>1078.6500000000001</v>
       </c>
-      <c r="AF2" s="5"/>
+      <c r="AE2" s="4">
+        <v>42748</v>
+      </c>
+      <c r="AF2" s="19">
+        <v>852.56</v>
+      </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B3" s="5"/>
@@ -1105,7 +1173,7 @@
       <c r="W32" s="5"/>
       <c r="Z32" s="5"/>
     </row>
-    <row r="33" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
       <c r="E33" s="5"/>
       <c r="H33" s="5"/>
@@ -1116,7 +1184,7 @@
       <c r="W33" s="5"/>
       <c r="Z33" s="5"/>
     </row>
-    <row r="34" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="E34" s="5"/>
       <c r="H34" s="5"/>
@@ -1127,7 +1195,7 @@
       <c r="W34" s="5"/>
       <c r="Z34" s="5"/>
     </row>
-    <row r="35" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
       <c r="E35" s="5"/>
       <c r="H35" s="5"/>
@@ -1138,7 +1206,7 @@
       <c r="W35" s="5"/>
       <c r="Z35" s="5"/>
     </row>
-    <row r="36" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>
       <c r="E36" s="5"/>
       <c r="H36" s="5"/>
@@ -1149,7 +1217,7 @@
       <c r="W36" s="5"/>
       <c r="Z36" s="5"/>
     </row>
-    <row r="37" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B37" s="5"/>
       <c r="E37" s="5"/>
       <c r="H37" s="5"/>
@@ -1160,7 +1228,7 @@
       <c r="W37" s="5"/>
       <c r="Z37" s="5"/>
     </row>
-    <row r="38" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B38" s="5"/>
       <c r="E38" s="5"/>
       <c r="H38" s="5"/>
@@ -1171,7 +1239,7 @@
       <c r="W38" s="5"/>
       <c r="Z38" s="5"/>
     </row>
-    <row r="39" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B39" s="5"/>
       <c r="E39" s="5"/>
       <c r="H39" s="5"/>
@@ -1182,7 +1250,7 @@
       <c r="W39" s="5"/>
       <c r="Z39" s="5"/>
     </row>
-    <row r="40" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B40" s="19">
         <f>SUM(B2:B39)</f>
         <v>1038.4000000000001</v>
@@ -1222,6 +1290,32 @@
       <c r="AC40" s="19">
         <f>SUM(AC2:AC39)</f>
         <v>1078.6500000000001</v>
+      </c>
+      <c r="AF40">
+        <f>SUM(AF2:AF39)</f>
+        <v>852.56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" s="25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>42748</v>
+      </c>
+      <c r="B43" s="19">
+        <v>1042.68</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" s="19">
+        <f>SUM(B43:B82)</f>
+        <v>1042.68</v>
       </c>
     </row>
   </sheetData>
@@ -1235,7 +1329,7 @@
   <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2048,17 +2142,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V12"/>
+  <dimension ref="A1:V14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -2076,7 +2170,7 @@
     <col min="18" max="18" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="7" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2100,49 +2194,49 @@
         <v>19</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" s="12">
-        <v>42370</v>
-      </c>
-      <c r="I1" s="12">
-        <v>42401</v>
-      </c>
-      <c r="J1" s="12">
-        <v>42430</v>
-      </c>
-      <c r="K1" s="12">
-        <v>42461</v>
-      </c>
-      <c r="L1" s="12">
-        <v>42491</v>
-      </c>
-      <c r="M1" s="12">
-        <v>42522</v>
-      </c>
-      <c r="N1" s="12">
-        <v>42552</v>
-      </c>
-      <c r="O1" s="12">
-        <v>42583</v>
-      </c>
-      <c r="P1" s="12">
-        <v>42614</v>
-      </c>
-      <c r="Q1" s="12">
-        <v>42644</v>
-      </c>
-      <c r="R1" s="12">
-        <v>42675</v>
-      </c>
-      <c r="S1" s="12">
-        <v>42705</v>
+        <v>52</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>49</v>
       </c>
       <c r="T1" s="11" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="U1" s="11" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="V1" s="10" t="s">
         <v>5</v>
@@ -2161,8 +2255,8 @@
       <c r="D2" s="8">
         <v>22.087</v>
       </c>
-      <c r="E2" s="20">
-        <f>V2/D2</f>
+      <c r="E2" s="33">
+        <f t="shared" ref="E2:E11" si="0">V2/D2</f>
         <v>47.190655136505647</v>
       </c>
       <c r="F2" s="9">
@@ -2218,7 +2312,7 @@
         <v>3.9</v>
       </c>
       <c r="V2" s="15">
-        <f>SUM(F2, U2)</f>
+        <f t="shared" ref="V2:V11" si="1">SUM(F2, U2)</f>
         <v>1042.3000000000002</v>
       </c>
     </row>
@@ -2235,8 +2329,8 @@
       <c r="D3" s="6">
         <v>8.1039999999999992</v>
       </c>
-      <c r="E3" s="22">
-        <f>V3/D3</f>
+      <c r="E3" s="34">
+        <f t="shared" si="0"/>
         <v>136.04639684106616</v>
       </c>
       <c r="F3" s="7">
@@ -2284,15 +2378,15 @@
         <v>0</v>
       </c>
       <c r="T3" s="18">
-        <f t="shared" ref="T3:T11" si="0">SUM(H3:S3)</f>
+        <f t="shared" ref="T3:T11" si="2">SUM(H3:S3)</f>
         <v>0</v>
       </c>
       <c r="U3" s="18">
-        <f t="shared" ref="U3:U11" si="1">SUM(G3:S3)</f>
+        <f t="shared" ref="U3:U11" si="3">SUM(G3:S3)</f>
         <v>12.84</v>
       </c>
       <c r="V3" s="16">
-        <f>SUM(F3, U3)</f>
+        <f t="shared" si="1"/>
         <v>1102.52</v>
       </c>
     </row>
@@ -2309,8 +2403,8 @@
       <c r="D4" s="8">
         <v>20.352</v>
       </c>
-      <c r="E4" s="20">
-        <f>V4/D4</f>
+      <c r="E4" s="33">
+        <f t="shared" si="0"/>
         <v>50.068297955974842</v>
       </c>
       <c r="F4" s="9">
@@ -2358,15 +2452,15 @@
         <v>0</v>
       </c>
       <c r="T4" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U4" s="17">
+        <f t="shared" si="3"/>
+        <v>19.189999999999998</v>
+      </c>
+      <c r="V4" s="15">
         <f t="shared" si="1"/>
-        <v>19.189999999999998</v>
-      </c>
-      <c r="V4" s="15">
-        <f>SUM(F4, U4)</f>
         <v>1018.99</v>
       </c>
     </row>
@@ -2383,8 +2477,8 @@
       <c r="D5" s="6">
         <v>19.152999999999999</v>
       </c>
-      <c r="E5" s="22">
-        <f>V5/D5</f>
+      <c r="E5" s="34">
+        <f t="shared" si="0"/>
         <v>35.395499399571868</v>
       </c>
       <c r="F5" s="7">
@@ -2432,15 +2526,15 @@
         <v>0</v>
       </c>
       <c r="T5" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U5" s="18">
+        <f t="shared" si="3"/>
+        <v>5.52</v>
+      </c>
+      <c r="V5" s="16">
         <f t="shared" si="1"/>
-        <v>5.52</v>
-      </c>
-      <c r="V5" s="16">
-        <f>SUM(F5, U5)</f>
         <v>677.93</v>
       </c>
     </row>
@@ -2457,8 +2551,8 @@
       <c r="D6" s="8">
         <v>9.125</v>
       </c>
-      <c r="E6" s="20">
-        <f>V6/D6</f>
+      <c r="E6" s="33">
+        <f t="shared" si="0"/>
         <v>118.76383561643836</v>
       </c>
       <c r="F6" s="9">
@@ -2506,15 +2600,15 @@
         <v>0</v>
       </c>
       <c r="T6" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U6" s="17">
+        <f t="shared" si="3"/>
+        <v>14.43</v>
+      </c>
+      <c r="V6" s="15">
         <f t="shared" si="1"/>
-        <v>14.43</v>
-      </c>
-      <c r="V6" s="15">
-        <f>SUM(F6, U6)</f>
         <v>1083.72</v>
       </c>
     </row>
@@ -2531,8 +2625,8 @@
       <c r="D7" s="6">
         <v>10.07</v>
       </c>
-      <c r="E7" s="22">
-        <f>V7/D7</f>
+      <c r="E7" s="34">
+        <f t="shared" si="0"/>
         <v>87.841112214498509</v>
       </c>
       <c r="F7" s="7">
@@ -2580,15 +2674,15 @@
         <v>0</v>
       </c>
       <c r="T7" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U7" s="18">
+        <f t="shared" si="3"/>
+        <v>5.96</v>
+      </c>
+      <c r="V7" s="16">
         <f t="shared" si="1"/>
-        <v>5.96</v>
-      </c>
-      <c r="V7" s="16">
-        <f>SUM(F7, U7)</f>
         <v>884.56000000000006</v>
       </c>
     </row>
@@ -2605,8 +2699,8 @@
       <c r="D8" s="8">
         <v>8.1240000000000006</v>
       </c>
-      <c r="E8" s="20">
-        <f>V8/D8</f>
+      <c r="E8" s="33">
+        <f t="shared" si="0"/>
         <v>118.49581486952239</v>
       </c>
       <c r="F8" s="9">
@@ -2654,15 +2748,15 @@
         <v>0</v>
       </c>
       <c r="T8" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U8" s="17">
+        <f t="shared" si="3"/>
+        <v>14.66</v>
+      </c>
+      <c r="V8" s="15">
         <f t="shared" si="1"/>
-        <v>14.66</v>
-      </c>
-      <c r="V8" s="15">
-        <f>SUM(F8, U8)</f>
         <v>962.66</v>
       </c>
     </row>
@@ -2677,11 +2771,11 @@
         <v>7</v>
       </c>
       <c r="D9" s="6">
-        <v>11</v>
-      </c>
-      <c r="E9" s="22">
-        <f>V9/D9</f>
-        <v>96.6</v>
+        <v>11.108000000000001</v>
+      </c>
+      <c r="E9" s="34">
+        <f t="shared" si="0"/>
+        <v>96.128015844436433</v>
       </c>
       <c r="F9" s="7">
         <f>'Initial Buys'!W40</f>
@@ -2692,7 +2786,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="24">
-        <v>0</v>
+        <v>5.19</v>
       </c>
       <c r="I9" s="21">
         <v>0</v>
@@ -2728,16 +2822,16 @@
         <v>0</v>
       </c>
       <c r="T9" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>5.19</v>
       </c>
       <c r="U9" s="18">
+        <f t="shared" si="3"/>
+        <v>5.19</v>
+      </c>
+      <c r="V9" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="V9" s="16">
-        <f>SUM(F9, U9)</f>
-        <v>1062.5999999999999</v>
+        <v>1067.79</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
@@ -2753,8 +2847,8 @@
       <c r="D10" s="8">
         <v>8.0470000000000006</v>
       </c>
-      <c r="E10" s="20">
-        <f>V10/D10</f>
+      <c r="E10" s="33">
+        <f t="shared" si="0"/>
         <v>136.60370324344476</v>
       </c>
       <c r="F10" s="9">
@@ -2802,165 +2896,311 @@
         <v>0</v>
       </c>
       <c r="T10" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U10" s="17">
+        <f t="shared" si="3"/>
+        <v>5.97</v>
+      </c>
+      <c r="V10" s="15">
         <f t="shared" si="1"/>
-        <v>5.97</v>
-      </c>
-      <c r="V10" s="15">
-        <f>SUM(F10, U10)</f>
         <v>1099.25</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="6">
+        <v>21</v>
+      </c>
+      <c r="E11" s="34">
+        <f>V11/D11</f>
+        <v>40.598095238095233</v>
+      </c>
+      <c r="F11" s="7">
+        <f>'Initial Buys'!AF40</f>
+        <v>852.56</v>
+      </c>
+      <c r="G11" s="27">
+        <v>0</v>
+      </c>
+      <c r="H11" s="24">
+        <v>0</v>
+      </c>
+      <c r="I11" s="21">
+        <v>0</v>
+      </c>
+      <c r="J11" s="24">
+        <v>0</v>
+      </c>
+      <c r="K11" s="21">
+        <v>0</v>
+      </c>
+      <c r="L11" s="24">
+        <v>0</v>
+      </c>
+      <c r="M11" s="21">
+        <v>0</v>
+      </c>
+      <c r="N11" s="24">
+        <v>0</v>
+      </c>
+      <c r="O11" s="21">
+        <v>0</v>
+      </c>
+      <c r="P11" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="21">
+        <v>0</v>
+      </c>
+      <c r="R11" s="24">
+        <v>0</v>
+      </c>
+      <c r="S11" s="21">
+        <v>0</v>
+      </c>
+      <c r="T11" s="18">
+        <f>SUM(H11:S11)</f>
+        <v>0</v>
+      </c>
+      <c r="U11" s="18">
+        <f>SUM(G11:S11)</f>
+        <v>0</v>
+      </c>
+      <c r="V11" s="16">
+        <f>SUM(F11, U11)</f>
+        <v>852.56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B12" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="6">
+      <c r="C12" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="8">
         <v>15.214</v>
       </c>
-      <c r="E11" s="22">
-        <f>V11/D11</f>
+      <c r="E12" s="33">
+        <f>V12/D12</f>
         <v>71.887734980938603</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F12" s="9">
         <f>'Initial Buys'!AC40</f>
         <v>1078.6500000000001</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G12" s="32">
         <f>'2016'!S11</f>
         <v>7.5</v>
       </c>
-      <c r="H11" s="24">
+      <c r="H12" s="24">
         <v>7.55</v>
       </c>
-      <c r="I11" s="21">
-        <v>0</v>
-      </c>
-      <c r="J11" s="24">
-        <v>0</v>
-      </c>
-      <c r="K11" s="21">
-        <v>0</v>
-      </c>
-      <c r="L11" s="24">
-        <v>0</v>
-      </c>
-      <c r="M11" s="21">
-        <v>0</v>
-      </c>
-      <c r="N11" s="24">
-        <v>0</v>
-      </c>
-      <c r="O11" s="21">
-        <v>0</v>
-      </c>
-      <c r="P11" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="21">
-        <v>0</v>
-      </c>
-      <c r="R11" s="24">
-        <v>0</v>
-      </c>
-      <c r="S11" s="21">
-        <v>0</v>
-      </c>
-      <c r="T11" s="18">
-        <f t="shared" si="0"/>
+      <c r="I12" s="21">
+        <v>0</v>
+      </c>
+      <c r="J12" s="24">
+        <v>0</v>
+      </c>
+      <c r="K12" s="21">
+        <v>0</v>
+      </c>
+      <c r="L12" s="24">
+        <v>0</v>
+      </c>
+      <c r="M12" s="21">
+        <v>0</v>
+      </c>
+      <c r="N12" s="24">
+        <v>0</v>
+      </c>
+      <c r="O12" s="21">
+        <v>0</v>
+      </c>
+      <c r="P12" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="21">
+        <v>0</v>
+      </c>
+      <c r="R12" s="24">
+        <v>0</v>
+      </c>
+      <c r="S12" s="21">
+        <v>0</v>
+      </c>
+      <c r="T12" s="17">
+        <f>SUM(H12:S12)</f>
         <v>7.55</v>
       </c>
-      <c r="U11" s="18">
-        <f t="shared" si="1"/>
+      <c r="U12" s="17">
+        <f>SUM(G12:S12)</f>
         <v>15.05</v>
       </c>
-      <c r="V11" s="16">
-        <f>SUM(F11, U11)</f>
+      <c r="V12" s="15">
+        <f>SUM(F12, U12)</f>
         <v>1093.7</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="29">
-        <f>SUM(F2:F11)</f>
-        <v>9930.7100000000009</v>
-      </c>
-      <c r="G12" s="30">
-        <f>SUM(G2:G11)</f>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="6">
+        <v>12</v>
+      </c>
+      <c r="E13" s="34">
+        <f t="shared" ref="E13" si="4">V13/D13</f>
+        <v>86.89</v>
+      </c>
+      <c r="F13" s="7">
+        <f>'Initial Buys'!B83</f>
+        <v>1042.68</v>
+      </c>
+      <c r="G13" s="27">
+        <v>0</v>
+      </c>
+      <c r="H13" s="24">
+        <v>0</v>
+      </c>
+      <c r="I13" s="21">
+        <v>0</v>
+      </c>
+      <c r="J13" s="24">
+        <v>0</v>
+      </c>
+      <c r="K13" s="21">
+        <v>0</v>
+      </c>
+      <c r="L13" s="24">
+        <v>0</v>
+      </c>
+      <c r="M13" s="21">
+        <v>0</v>
+      </c>
+      <c r="N13" s="24">
+        <v>0</v>
+      </c>
+      <c r="O13" s="21">
+        <v>0</v>
+      </c>
+      <c r="P13" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="21">
+        <v>0</v>
+      </c>
+      <c r="R13" s="24">
+        <v>0</v>
+      </c>
+      <c r="S13" s="21">
+        <v>0</v>
+      </c>
+      <c r="T13" s="18">
+        <f t="shared" ref="T13" si="5">SUM(H13:S13)</f>
+        <v>0</v>
+      </c>
+      <c r="U13" s="18">
+        <f t="shared" ref="U13" si="6">SUM(G13:S13)</f>
+        <v>0</v>
+      </c>
+      <c r="V13" s="16">
+        <f t="shared" ref="V13" si="7">SUM(F13, U13)</f>
+        <v>1042.68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="29">
+        <f>SUM(F2:F13)</f>
+        <v>11825.95</v>
+      </c>
+      <c r="G14" s="30">
+        <f>SUM(G2:G13)</f>
         <v>89.969999999999985</v>
       </c>
-      <c r="H12" s="31">
-        <f t="shared" ref="H12:S12" si="2">SUM(H2:H11)</f>
-        <v>7.55</v>
-      </c>
-      <c r="I12" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="31">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K12" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L12" s="31">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M12" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N12" s="31">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O12" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P12" s="31">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R12" s="31">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="S12" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T12" s="30">
-        <f>SUM(T2:T11)</f>
-        <v>7.55</v>
-      </c>
-      <c r="U12" s="30">
-        <f>SUM(U2:U11)</f>
-        <v>97.519999999999982</v>
-      </c>
-      <c r="V12" s="23">
-        <f>SUM(V2:V11)</f>
-        <v>10028.230000000001</v>
+      <c r="H14" s="31">
+        <f>SUM(H2:H13)</f>
+        <v>12.74</v>
+      </c>
+      <c r="I14" s="30">
+        <f>SUM(I2:I13)</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="31">
+        <f>SUM(J2:J13)</f>
+        <v>0</v>
+      </c>
+      <c r="K14" s="30">
+        <f>SUM(K2:K13)</f>
+        <v>0</v>
+      </c>
+      <c r="L14" s="31">
+        <f>SUM(L2:L13)</f>
+        <v>0</v>
+      </c>
+      <c r="M14" s="30">
+        <f>SUM(M2:M13)</f>
+        <v>0</v>
+      </c>
+      <c r="N14" s="31">
+        <f>SUM(N2:N13)</f>
+        <v>0</v>
+      </c>
+      <c r="O14" s="30">
+        <f>SUM(O2:O13)</f>
+        <v>0</v>
+      </c>
+      <c r="P14" s="31">
+        <f>SUM(P2:P13)</f>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="30">
+        <f>SUM(Q2:Q13)</f>
+        <v>0</v>
+      </c>
+      <c r="R14" s="31">
+        <f>SUM(R2:R13)</f>
+        <v>0</v>
+      </c>
+      <c r="S14" s="30">
+        <f>SUM(S2:S13)</f>
+        <v>0</v>
+      </c>
+      <c r="T14" s="30">
+        <f>SUM(T2:T13)</f>
+        <v>12.74</v>
+      </c>
+      <c r="U14" s="30">
+        <f>SUM(U2:U13)</f>
+        <v>102.70999999999998</v>
+      </c>
+      <c r="V14" s="23">
+        <f>SUM(V2:V13)</f>
+        <v>11928.660000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
udated excel and xml.
</commit_message>
<xml_diff>
--- a/DividendLiberty/401k.xlsx
+++ b/DividendLiberty/401k.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\Documents\GitHub\DividendLibertyCommercial\DividendLiberty\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steve Yi\Documents\GitHub\DividendLibertyCommercial\DividendLiberty\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -190,9 +190,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -340,8 +341,8 @@
     <xf numFmtId="2" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,23 +436,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -487,23 +471,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2145,7 +2112,7 @@
   <dimension ref="A1:V14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2256,7 +2223,7 @@
         <v>22.087</v>
       </c>
       <c r="E2" s="33">
-        <f t="shared" ref="E2:E11" si="0">V2/D2</f>
+        <f t="shared" ref="E2:E10" si="0">V2/D2</f>
         <v>47.190655136505647</v>
       </c>
       <c r="F2" s="9">
@@ -2312,7 +2279,7 @@
         <v>3.9</v>
       </c>
       <c r="V2" s="15">
-        <f t="shared" ref="V2:V11" si="1">SUM(F2, U2)</f>
+        <f t="shared" ref="V2:V10" si="1">SUM(F2, U2)</f>
         <v>1042.3000000000002</v>
       </c>
     </row>
@@ -2378,11 +2345,11 @@
         <v>0</v>
       </c>
       <c r="T3" s="18">
-        <f t="shared" ref="T3:T11" si="2">SUM(H3:S3)</f>
+        <f t="shared" ref="T3:T10" si="2">SUM(H3:S3)</f>
         <v>0</v>
       </c>
       <c r="U3" s="18">
-        <f t="shared" ref="U3:U11" si="3">SUM(G3:S3)</f>
+        <f t="shared" ref="U3:U10" si="3">SUM(G3:S3)</f>
         <v>12.84</v>
       </c>
       <c r="V3" s="16">
@@ -3135,71 +3102,71 @@
       <c r="D14" s="28"/>
       <c r="E14" s="28"/>
       <c r="F14" s="29">
-        <f>SUM(F2:F13)</f>
+        <f t="shared" ref="F14:V14" si="8">SUM(F2:F13)</f>
         <v>11825.95</v>
       </c>
       <c r="G14" s="30">
-        <f>SUM(G2:G13)</f>
+        <f t="shared" si="8"/>
         <v>89.969999999999985</v>
       </c>
       <c r="H14" s="31">
-        <f>SUM(H2:H13)</f>
+        <f t="shared" si="8"/>
         <v>12.74</v>
       </c>
       <c r="I14" s="30">
-        <f>SUM(I2:I13)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J14" s="31">
-        <f>SUM(J2:J13)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K14" s="30">
-        <f>SUM(K2:K13)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L14" s="31">
-        <f>SUM(L2:L13)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="M14" s="30">
-        <f>SUM(M2:M13)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="N14" s="31">
-        <f>SUM(N2:N13)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O14" s="30">
-        <f>SUM(O2:O13)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P14" s="31">
-        <f>SUM(P2:P13)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q14" s="30">
-        <f>SUM(Q2:Q13)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="R14" s="31">
-        <f>SUM(R2:R13)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="S14" s="30">
-        <f>SUM(S2:S13)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="T14" s="30">
-        <f>SUM(T2:T13)</f>
+        <f t="shared" si="8"/>
         <v>12.74</v>
       </c>
       <c r="U14" s="30">
-        <f>SUM(U2:U13)</f>
+        <f t="shared" si="8"/>
         <v>102.70999999999998</v>
       </c>
       <c r="V14" s="23">
-        <f>SUM(V2:V13)</f>
+        <f t="shared" si="8"/>
         <v>11928.660000000002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated excel taxable and total dividends again.
</commit_message>
<xml_diff>
--- a/DividendLiberty/401k.xlsx
+++ b/DividendLiberty/401k.xlsx
@@ -2146,7 +2146,7 @@
   <dimension ref="A1:V14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2993,11 +2993,11 @@
         <v>7</v>
       </c>
       <c r="D12" s="8">
-        <v>15.214</v>
+        <v>15.324</v>
       </c>
       <c r="E12" s="33">
         <f>V12/D12</f>
-        <v>71.887734980938603</v>
+        <v>71.878099712868703</v>
       </c>
       <c r="F12" s="9">
         <f>'Initial Buys'!AC40</f>
@@ -3017,7 +3017,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="21">
-        <v>0</v>
+        <v>7.76</v>
       </c>
       <c r="L12" s="24">
         <v>0</v>
@@ -3045,15 +3045,15 @@
       </c>
       <c r="T12" s="17">
         <f>SUM(H12:S12)</f>
-        <v>7.55</v>
+        <v>15.309999999999999</v>
       </c>
       <c r="U12" s="17">
         <f>SUM(G12:S12)</f>
-        <v>15.05</v>
+        <v>22.810000000000002</v>
       </c>
       <c r="V12" s="15">
         <f>SUM(F12, U12)</f>
-        <v>1093.7</v>
+        <v>1101.46</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
@@ -3157,7 +3157,7 @@
       </c>
       <c r="K14" s="30">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>7.76</v>
       </c>
       <c r="L14" s="31">
         <f t="shared" si="8"/>
@@ -3193,15 +3193,15 @@
       </c>
       <c r="T14" s="30">
         <f t="shared" si="8"/>
-        <v>72.47</v>
+        <v>80.23</v>
       </c>
       <c r="U14" s="30">
         <f t="shared" si="8"/>
-        <v>162.44</v>
+        <v>170.2</v>
       </c>
       <c r="V14" s="23">
         <f t="shared" si="8"/>
-        <v>11988.390000000001</v>
+        <v>11996.150000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated excel and xml
</commit_message>
<xml_diff>
--- a/DividendLiberty/401k.xlsx
+++ b/DividendLiberty/401k.xlsx
@@ -2112,7 +2112,7 @@
   <dimension ref="A1:V14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2516,11 +2516,11 @@
         <v>7</v>
       </c>
       <c r="D6" s="8">
-        <v>9.1829999999999998</v>
+        <v>9.2420000000000009</v>
       </c>
       <c r="E6" s="33">
         <f t="shared" si="0"/>
-        <v>118.80866819122291</v>
+        <v>118.88444059727331</v>
       </c>
       <c r="F6" s="9">
         <f>'Initial Buys'!N40</f>
@@ -2546,7 +2546,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="21">
-        <v>0</v>
+        <v>7.71</v>
       </c>
       <c r="N6" s="24">
         <v>0</v>
@@ -2568,15 +2568,15 @@
       </c>
       <c r="T6" s="17">
         <f t="shared" si="2"/>
-        <v>7.3</v>
+        <v>15.01</v>
       </c>
       <c r="U6" s="17">
         <f t="shared" si="3"/>
-        <v>21.73</v>
+        <v>29.44</v>
       </c>
       <c r="V6" s="15">
         <f t="shared" si="1"/>
-        <v>1091.02</v>
+        <v>1098.73</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -3131,7 +3131,7 @@
       </c>
       <c r="M14" s="30">
         <f t="shared" si="8"/>
-        <v>37.269999999999996</v>
+        <v>44.98</v>
       </c>
       <c r="N14" s="31">
         <f t="shared" si="8"/>
@@ -3159,15 +3159,15 @@
       </c>
       <c r="T14" s="30">
         <f t="shared" si="8"/>
-        <v>142.79999999999998</v>
+        <v>150.51</v>
       </c>
       <c r="U14" s="30">
         <f t="shared" si="8"/>
-        <v>232.76999999999995</v>
+        <v>240.48</v>
       </c>
       <c r="V14" s="23">
         <f t="shared" si="8"/>
-        <v>12058.720000000001</v>
+        <v>12066.430000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated excel sheet 401k and total dividends.
</commit_message>
<xml_diff>
--- a/DividendLiberty/401k.xlsx
+++ b/DividendLiberty/401k.xlsx
@@ -2123,7 +2123,7 @@
   <dimension ref="A1:V14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2675,11 +2675,11 @@
         <v>31</v>
       </c>
       <c r="D8" s="8">
-        <v>8.1839999999999993</v>
+        <v>8.2349999999999994</v>
       </c>
       <c r="E8" s="33">
         <f t="shared" si="0"/>
-        <v>118.56060606060606</v>
+        <v>118.76017000607166</v>
       </c>
       <c r="F8" s="9">
         <f>'Initial Buys'!T40</f>
@@ -2705,7 +2705,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="21">
-        <v>0</v>
+        <v>7.69</v>
       </c>
       <c r="N8" s="24">
         <v>0</v>
@@ -2727,15 +2727,15 @@
       </c>
       <c r="T8" s="17">
         <f t="shared" si="2"/>
-        <v>7.64</v>
+        <v>15.33</v>
       </c>
       <c r="U8" s="17">
         <f t="shared" si="3"/>
-        <v>22.3</v>
+        <v>29.990000000000002</v>
       </c>
       <c r="V8" s="15">
         <f t="shared" si="1"/>
-        <v>970.3</v>
+        <v>977.99</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -3142,7 +3142,7 @@
       </c>
       <c r="M14" s="30">
         <f t="shared" si="8"/>
-        <v>51.06</v>
+        <v>58.75</v>
       </c>
       <c r="N14" s="31">
         <f t="shared" si="8"/>
@@ -3170,15 +3170,15 @@
       </c>
       <c r="T14" s="30">
         <f t="shared" si="8"/>
-        <v>156.58999999999997</v>
+        <v>164.27999999999997</v>
       </c>
       <c r="U14" s="30">
         <f t="shared" si="8"/>
-        <v>246.55999999999997</v>
+        <v>254.24999999999997</v>
       </c>
       <c r="V14" s="23">
         <f t="shared" si="8"/>
-        <v>13056.890000000001</v>
+        <v>13064.580000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated excel and xml, no more taxable account
</commit_message>
<xml_diff>
--- a/DividendLiberty/401k.xlsx
+++ b/DividendLiberty/401k.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="63">
   <si>
     <t>Symbols</t>
   </si>
@@ -185,17 +185,48 @@
   </si>
   <si>
     <t>Prev All Time Dividends</t>
+  </si>
+  <si>
+    <t>DIS</t>
+  </si>
+  <si>
+    <t>Disney Walt Co</t>
+  </si>
+  <si>
+    <t>Consumer Discretionary</t>
+  </si>
+  <si>
+    <t>SO</t>
+  </si>
+  <si>
+    <t>MMM</t>
+  </si>
+  <si>
+    <t>PEP</t>
+  </si>
+  <si>
+    <t>Southern Co</t>
+  </si>
+  <si>
+    <t>Pepsico Inc</t>
+  </si>
+  <si>
+    <t>3M Company</t>
+  </si>
+  <si>
+    <t>Utilities</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="170" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,6 +260,12 @@
       <b/>
       <sz val="10"/>
       <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333A42"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -301,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -343,6 +380,8 @@
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF83"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,18 +673,15 @@
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="4.42578125" bestFit="1" customWidth="1"/>
@@ -1281,6 +1317,30 @@
       <c r="B42" s="25" t="s">
         <v>37</v>
       </c>
+      <c r="E42" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I42" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L42" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="N42" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O42" s="25" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="43" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
@@ -1289,11 +1349,59 @@
       <c r="B43" s="19">
         <v>1042.68</v>
       </c>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="E43" s="4">
+        <v>42912</v>
+      </c>
+      <c r="F43" s="19">
+        <v>946.8</v>
+      </c>
+      <c r="H43" s="4">
+        <v>42912</v>
+      </c>
+      <c r="I43" s="19">
+        <v>999.4</v>
+      </c>
+      <c r="K43" s="4">
+        <v>42912</v>
+      </c>
+      <c r="L43" s="19">
+        <v>851.92</v>
+      </c>
+      <c r="N43" s="4">
+        <v>42912</v>
+      </c>
+      <c r="O43" s="19">
+        <v>1055.7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="N44" s="4">
+        <v>42912</v>
+      </c>
+      <c r="O44" s="35">
+        <v>117.617</v>
+      </c>
+    </row>
+    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B83" s="19">
         <f>SUM(B43:B82)</f>
         <v>1042.68</v>
+      </c>
+      <c r="F83" s="19">
+        <f>SUM(F43:F82)</f>
+        <v>946.8</v>
+      </c>
+      <c r="I83" s="19">
+        <f>SUM(I43:I82)</f>
+        <v>999.4</v>
+      </c>
+      <c r="L83" s="19">
+        <f>SUM(L43:L82)</f>
+        <v>851.92</v>
+      </c>
+      <c r="O83" s="19">
+        <f>SUM(O43:O82)</f>
+        <v>1173.317</v>
       </c>
     </row>
   </sheetData>
@@ -2120,17 +2228,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V14"/>
+  <dimension ref="A1:V18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -2234,7 +2342,7 @@
         <v>22.254000000000001</v>
       </c>
       <c r="E2" s="33">
-        <f t="shared" ref="E2:E10" si="0">V2/D2</f>
+        <f t="shared" ref="E2:E14" si="0">V2/D2</f>
         <v>47.214433360294777</v>
       </c>
       <c r="F2" s="9">
@@ -2290,7 +2398,7 @@
         <v>12.309999999999999</v>
       </c>
       <c r="V2" s="15">
-        <f t="shared" ref="V2:V10" si="1">SUM(F2, U2)</f>
+        <f t="shared" ref="V2:V14" si="1">SUM(F2, U2)</f>
         <v>1050.71</v>
       </c>
     </row>
@@ -2356,829 +2464,1121 @@
         <v>0</v>
       </c>
       <c r="T3" s="18">
-        <f t="shared" ref="T3:T10" si="2">SUM(H3:S3)</f>
+        <f t="shared" ref="T3:T14" si="2">SUM(H3:S3)</f>
         <v>13</v>
       </c>
       <c r="U3" s="18">
-        <f t="shared" ref="U3:U10" si="3">SUM(G3:S3)</f>
+        <f t="shared" ref="U3:U14" si="3">SUM(G3:S3)</f>
         <v>25.84</v>
       </c>
       <c r="V3" s="16">
-        <f t="shared" si="1"/>
+        <f>SUM(F3, U3)</f>
         <v>1115.52</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="8">
         <v>9</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="8">
-        <v>20.681999999999999</v>
       </c>
       <c r="E4" s="33">
         <f t="shared" si="0"/>
+        <v>105.19999999999999</v>
+      </c>
+      <c r="F4" s="9">
+        <f>'Initial Buys'!F83</f>
+        <v>946.8</v>
+      </c>
+      <c r="G4" s="32">
+        <v>0</v>
+      </c>
+      <c r="H4" s="24">
+        <v>0</v>
+      </c>
+      <c r="I4" s="21">
+        <v>0</v>
+      </c>
+      <c r="J4" s="24">
+        <v>0</v>
+      </c>
+      <c r="K4" s="21">
+        <v>0</v>
+      </c>
+      <c r="L4" s="24">
+        <v>0</v>
+      </c>
+      <c r="M4" s="21">
+        <v>0</v>
+      </c>
+      <c r="N4" s="24">
+        <v>0</v>
+      </c>
+      <c r="O4" s="21">
+        <v>0</v>
+      </c>
+      <c r="P4" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="21">
+        <v>0</v>
+      </c>
+      <c r="R4" s="24">
+        <v>0</v>
+      </c>
+      <c r="S4" s="21">
+        <v>0</v>
+      </c>
+      <c r="T4" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U4" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V4" s="15">
+        <f>SUM(F4, U4)</f>
+        <v>946.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="6">
+        <v>20.681999999999999</v>
+      </c>
+      <c r="E5" s="34">
+        <f t="shared" si="0"/>
         <v>50.218064017019628</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F5" s="7">
         <f>'Initial Buys'!H40</f>
         <v>999.8</v>
       </c>
-      <c r="G4" s="26">
+      <c r="G5" s="27">
         <f>'2016'!S4</f>
         <v>19.189999999999998</v>
       </c>
-      <c r="H4" s="24">
-        <v>0</v>
-      </c>
-      <c r="I4" s="21">
-        <v>0</v>
-      </c>
-      <c r="J4" s="24">
+      <c r="H5" s="24">
+        <v>0</v>
+      </c>
+      <c r="I5" s="21">
+        <v>0</v>
+      </c>
+      <c r="J5" s="24">
         <v>9.77</v>
       </c>
-      <c r="K4" s="21">
-        <v>0</v>
-      </c>
-      <c r="L4" s="24">
-        <v>0</v>
-      </c>
-      <c r="M4" s="21">
+      <c r="K5" s="21">
+        <v>0</v>
+      </c>
+      <c r="L5" s="24">
+        <v>0</v>
+      </c>
+      <c r="M5" s="21">
         <v>9.85</v>
       </c>
-      <c r="N4" s="24">
-        <v>0</v>
-      </c>
-      <c r="O4" s="21">
-        <v>0</v>
-      </c>
-      <c r="P4" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="21">
-        <v>0</v>
-      </c>
-      <c r="R4" s="24">
-        <v>0</v>
-      </c>
-      <c r="S4" s="21">
-        <v>0</v>
-      </c>
-      <c r="T4" s="17">
+      <c r="N5" s="24">
+        <v>0</v>
+      </c>
+      <c r="O5" s="21">
+        <v>0</v>
+      </c>
+      <c r="P5" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="21">
+        <v>0</v>
+      </c>
+      <c r="R5" s="24">
+        <v>0</v>
+      </c>
+      <c r="S5" s="21">
+        <v>0</v>
+      </c>
+      <c r="T5" s="18">
         <f t="shared" si="2"/>
         <v>19.619999999999997</v>
       </c>
-      <c r="U4" s="17">
+      <c r="U5" s="18">
         <f t="shared" si="3"/>
         <v>38.809999999999995</v>
       </c>
-      <c r="V4" s="15">
+      <c r="V5" s="16">
         <f t="shared" si="1"/>
         <v>1038.6099999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D6" s="8">
         <v>33.335999999999999</v>
       </c>
-      <c r="E5" s="34">
+      <c r="E6" s="33">
         <f t="shared" si="0"/>
         <v>34.953803695704345</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F6" s="9">
         <f>'Initial Buys'!K40</f>
         <v>1153.17</v>
       </c>
-      <c r="G5" s="27">
+      <c r="G6" s="32">
         <f>'2016'!S5</f>
         <v>5.52</v>
       </c>
-      <c r="H5" s="24">
-        <v>0</v>
-      </c>
-      <c r="I5" s="21">
+      <c r="H6" s="24">
+        <v>0</v>
+      </c>
+      <c r="I6" s="21">
         <v>3.26</v>
       </c>
-      <c r="J5" s="24">
-        <v>0</v>
-      </c>
-      <c r="K5" s="21">
-        <v>0</v>
-      </c>
-      <c r="L5" s="24">
+      <c r="J6" s="24">
+        <v>0</v>
+      </c>
+      <c r="K6" s="21">
+        <v>0</v>
+      </c>
+      <c r="L6" s="24">
         <v>3.27</v>
       </c>
-      <c r="M5" s="21">
-        <v>0</v>
-      </c>
-      <c r="N5" s="24">
-        <v>0</v>
-      </c>
-      <c r="O5" s="21">
-        <v>0</v>
-      </c>
-      <c r="P5" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="21">
-        <v>0</v>
-      </c>
-      <c r="R5" s="24">
-        <v>0</v>
-      </c>
-      <c r="S5" s="21">
-        <v>0</v>
-      </c>
-      <c r="T5" s="18">
+      <c r="M6" s="21">
+        <v>0</v>
+      </c>
+      <c r="N6" s="24">
+        <v>0</v>
+      </c>
+      <c r="O6" s="21">
+        <v>0</v>
+      </c>
+      <c r="P6" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="21">
+        <v>0</v>
+      </c>
+      <c r="R6" s="24">
+        <v>0</v>
+      </c>
+      <c r="S6" s="21">
+        <v>0</v>
+      </c>
+      <c r="T6" s="17">
         <f t="shared" si="2"/>
         <v>6.5299999999999994</v>
       </c>
-      <c r="U5" s="18">
+      <c r="U6" s="17">
         <f t="shared" si="3"/>
         <v>12.049999999999999</v>
       </c>
-      <c r="V5" s="16">
+      <c r="V6" s="15">
         <f t="shared" si="1"/>
         <v>1165.22</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D7" s="6">
         <v>9.2420000000000009</v>
       </c>
-      <c r="E6" s="33">
+      <c r="E7" s="34">
         <f t="shared" si="0"/>
         <v>118.88444059727331</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F7" s="7">
         <f>'Initial Buys'!N40</f>
         <v>1069.29</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G7" s="27">
         <f>'2016'!S6</f>
         <v>14.43</v>
       </c>
-      <c r="H6" s="24">
-        <v>0</v>
-      </c>
-      <c r="I6" s="21">
-        <v>0</v>
-      </c>
-      <c r="J6" s="24">
+      <c r="H7" s="24">
+        <v>0</v>
+      </c>
+      <c r="I7" s="21">
+        <v>0</v>
+      </c>
+      <c r="J7" s="24">
         <v>7.3</v>
       </c>
-      <c r="K6" s="21">
-        <v>0</v>
-      </c>
-      <c r="L6" s="24">
-        <v>0</v>
-      </c>
-      <c r="M6" s="21">
+      <c r="K7" s="21">
+        <v>0</v>
+      </c>
+      <c r="L7" s="24">
+        <v>0</v>
+      </c>
+      <c r="M7" s="21">
         <v>7.71</v>
       </c>
-      <c r="N6" s="24">
-        <v>0</v>
-      </c>
-      <c r="O6" s="21">
-        <v>0</v>
-      </c>
-      <c r="P6" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="21">
-        <v>0</v>
-      </c>
-      <c r="R6" s="24">
-        <v>0</v>
-      </c>
-      <c r="S6" s="21">
-        <v>0</v>
-      </c>
-      <c r="T6" s="17">
+      <c r="N7" s="24">
+        <v>0</v>
+      </c>
+      <c r="O7" s="21">
+        <v>0</v>
+      </c>
+      <c r="P7" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="21">
+        <v>0</v>
+      </c>
+      <c r="R7" s="24">
+        <v>0</v>
+      </c>
+      <c r="S7" s="21">
+        <v>0</v>
+      </c>
+      <c r="T7" s="18">
         <f t="shared" si="2"/>
         <v>15.01</v>
       </c>
-      <c r="U6" s="17">
+      <c r="U7" s="18">
         <f t="shared" si="3"/>
         <v>29.44</v>
       </c>
-      <c r="V6" s="15">
+      <c r="V7" s="16">
         <f t="shared" si="1"/>
         <v>1098.73</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D8" s="8">
         <v>10.202999999999999</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E8" s="33">
         <f t="shared" si="0"/>
         <v>87.883955699304138</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F8" s="9">
         <f>'Initial Buys'!Q40</f>
         <v>878.6</v>
       </c>
-      <c r="G7" s="27">
+      <c r="G8" s="32">
         <f>'2016'!S7</f>
         <v>5.96</v>
       </c>
-      <c r="H7" s="24">
-        <v>0</v>
-      </c>
-      <c r="I7" s="21">
-        <v>0</v>
-      </c>
-      <c r="J7" s="24">
+      <c r="H8" s="24">
+        <v>0</v>
+      </c>
+      <c r="I8" s="21">
+        <v>0</v>
+      </c>
+      <c r="J8" s="24">
         <v>6.04</v>
       </c>
-      <c r="K7" s="21">
-        <v>0</v>
-      </c>
-      <c r="L7" s="24">
-        <v>0</v>
-      </c>
-      <c r="M7" s="21">
+      <c r="K8" s="21">
+        <v>0</v>
+      </c>
+      <c r="L8" s="24">
+        <v>0</v>
+      </c>
+      <c r="M8" s="21">
         <v>6.08</v>
       </c>
-      <c r="N7" s="24">
-        <v>0</v>
-      </c>
-      <c r="O7" s="21">
-        <v>0</v>
-      </c>
-      <c r="P7" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="21">
-        <v>0</v>
-      </c>
-      <c r="R7" s="24">
-        <v>0</v>
-      </c>
-      <c r="S7" s="21">
-        <v>0</v>
-      </c>
-      <c r="T7" s="18">
+      <c r="N8" s="24">
+        <v>0</v>
+      </c>
+      <c r="O8" s="21">
+        <v>0</v>
+      </c>
+      <c r="P8" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="21">
+        <v>0</v>
+      </c>
+      <c r="R8" s="24">
+        <v>0</v>
+      </c>
+      <c r="S8" s="21">
+        <v>0</v>
+      </c>
+      <c r="T8" s="17">
         <f t="shared" si="2"/>
         <v>12.120000000000001</v>
       </c>
-      <c r="U7" s="18">
+      <c r="U8" s="17">
         <f t="shared" si="3"/>
         <v>18.079999999999998</v>
       </c>
-      <c r="V7" s="16">
+      <c r="V8" s="15">
         <f t="shared" si="1"/>
         <v>896.68000000000006</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D9" s="6">
         <v>8.2349999999999994</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E9" s="34">
         <f t="shared" si="0"/>
         <v>118.76017000607166</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F9" s="7">
         <f>'Initial Buys'!T40</f>
         <v>948</v>
       </c>
-      <c r="G8" s="26">
+      <c r="G9" s="27">
         <f>'2016'!S8</f>
         <v>14.66</v>
       </c>
-      <c r="H8" s="24">
-        <v>0</v>
-      </c>
-      <c r="I8" s="21">
-        <v>0</v>
-      </c>
-      <c r="J8" s="24">
+      <c r="H9" s="24">
+        <v>0</v>
+      </c>
+      <c r="I9" s="21">
+        <v>0</v>
+      </c>
+      <c r="J9" s="24">
         <v>7.64</v>
       </c>
-      <c r="K8" s="21">
-        <v>0</v>
-      </c>
-      <c r="L8" s="24">
-        <v>0</v>
-      </c>
-      <c r="M8" s="21">
+      <c r="K9" s="21">
+        <v>0</v>
+      </c>
+      <c r="L9" s="24">
+        <v>0</v>
+      </c>
+      <c r="M9" s="21">
         <v>7.69</v>
       </c>
-      <c r="N8" s="24">
-        <v>0</v>
-      </c>
-      <c r="O8" s="21">
-        <v>0</v>
-      </c>
-      <c r="P8" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="21">
-        <v>0</v>
-      </c>
-      <c r="R8" s="24">
-        <v>0</v>
-      </c>
-      <c r="S8" s="21">
-        <v>0</v>
-      </c>
-      <c r="T8" s="17">
+      <c r="N9" s="24">
+        <v>0</v>
+      </c>
+      <c r="O9" s="21">
+        <v>0</v>
+      </c>
+      <c r="P9" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="21">
+        <v>0</v>
+      </c>
+      <c r="R9" s="24">
+        <v>0</v>
+      </c>
+      <c r="S9" s="21">
+        <v>0</v>
+      </c>
+      <c r="T9" s="18">
         <f t="shared" si="2"/>
         <v>15.33</v>
       </c>
-      <c r="U8" s="17">
+      <c r="U9" s="18">
         <f t="shared" si="3"/>
         <v>29.990000000000002</v>
       </c>
-      <c r="V8" s="15">
+      <c r="V9" s="16">
         <f t="shared" si="1"/>
         <v>977.99</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B10" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D10" s="8">
         <v>11.16</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E10" s="33">
         <f t="shared" si="0"/>
         <v>96.147849462365585</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F10" s="9">
         <f>'Initial Buys'!W40</f>
         <v>1062.5999999999999</v>
       </c>
-      <c r="G9" s="27">
+      <c r="G10" s="32">
         <f>'2016'!S9</f>
         <v>0</v>
       </c>
-      <c r="H9" s="24">
+      <c r="H10" s="24">
         <v>5.19</v>
       </c>
-      <c r="I9" s="21">
-        <v>0</v>
-      </c>
-      <c r="J9" s="24">
-        <v>0</v>
-      </c>
-      <c r="K9" s="21">
+      <c r="I10" s="21">
+        <v>0</v>
+      </c>
+      <c r="J10" s="24">
+        <v>0</v>
+      </c>
+      <c r="K10" s="21">
         <v>5.22</v>
       </c>
-      <c r="L9" s="24">
-        <v>0</v>
-      </c>
-      <c r="M9" s="21">
-        <v>0</v>
-      </c>
-      <c r="N9" s="24">
-        <v>0</v>
-      </c>
-      <c r="O9" s="21">
-        <v>0</v>
-      </c>
-      <c r="P9" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="21">
-        <v>0</v>
-      </c>
-      <c r="R9" s="24">
-        <v>0</v>
-      </c>
-      <c r="S9" s="21">
-        <v>0</v>
-      </c>
-      <c r="T9" s="18">
+      <c r="L10" s="24">
+        <v>0</v>
+      </c>
+      <c r="M10" s="21">
+        <v>0</v>
+      </c>
+      <c r="N10" s="24">
+        <v>0</v>
+      </c>
+      <c r="O10" s="21">
+        <v>0</v>
+      </c>
+      <c r="P10" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="21">
+        <v>0</v>
+      </c>
+      <c r="R10" s="24">
+        <v>0</v>
+      </c>
+      <c r="S10" s="21">
+        <v>0</v>
+      </c>
+      <c r="T10" s="17">
         <f t="shared" si="2"/>
         <v>10.41</v>
       </c>
-      <c r="U9" s="18">
+      <c r="U10" s="17">
         <f t="shared" si="3"/>
         <v>10.41</v>
       </c>
-      <c r="V9" s="16">
+      <c r="V10" s="15">
         <f t="shared" si="1"/>
         <v>1073.01</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="6">
+        <v>4</v>
+      </c>
+      <c r="E11" s="34">
+        <f t="shared" si="0"/>
+        <v>212.98</v>
+      </c>
+      <c r="F11" s="7">
+        <f>'Initial Buys'!L83</f>
+        <v>851.92</v>
+      </c>
+      <c r="G11" s="27">
+        <v>0</v>
+      </c>
+      <c r="H11" s="24">
+        <v>0</v>
+      </c>
+      <c r="I11" s="21">
+        <v>0</v>
+      </c>
+      <c r="J11" s="24">
+        <v>0</v>
+      </c>
+      <c r="K11" s="21">
+        <v>0</v>
+      </c>
+      <c r="L11" s="24">
+        <v>0</v>
+      </c>
+      <c r="M11" s="21">
+        <v>0</v>
+      </c>
+      <c r="N11" s="24">
+        <v>0</v>
+      </c>
+      <c r="O11" s="21">
+        <v>0</v>
+      </c>
+      <c r="P11" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="21">
+        <v>0</v>
+      </c>
+      <c r="R11" s="24">
+        <v>0</v>
+      </c>
+      <c r="S11" s="21">
+        <v>0</v>
+      </c>
+      <c r="T11" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U11" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V11" s="16">
+        <f t="shared" si="1"/>
+        <v>851.92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="8">
+        <v>10</v>
+      </c>
+      <c r="E12" s="33">
+        <f t="shared" si="0"/>
+        <v>117.3317</v>
+      </c>
+      <c r="F12" s="9">
+        <f>'Initial Buys'!O83</f>
+        <v>1173.317</v>
+      </c>
+      <c r="G12" s="32">
+        <v>0</v>
+      </c>
+      <c r="H12" s="24">
+        <v>0</v>
+      </c>
+      <c r="I12" s="21">
+        <v>0</v>
+      </c>
+      <c r="J12" s="24">
+        <v>0</v>
+      </c>
+      <c r="K12" s="21">
+        <v>0</v>
+      </c>
+      <c r="L12" s="24">
+        <v>0</v>
+      </c>
+      <c r="M12" s="21">
+        <v>0</v>
+      </c>
+      <c r="N12" s="24">
+        <v>0</v>
+      </c>
+      <c r="O12" s="21">
+        <v>0</v>
+      </c>
+      <c r="P12" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="21">
+        <v>0</v>
+      </c>
+      <c r="R12" s="24">
+        <v>0</v>
+      </c>
+      <c r="S12" s="21">
+        <v>0</v>
+      </c>
+      <c r="T12" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U12" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V12" s="15">
+        <f t="shared" si="1"/>
+        <v>1173.317</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B13" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D13" s="6">
         <v>8.1370000000000005</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E13" s="34">
         <f t="shared" si="0"/>
         <v>136.58104952685264</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F13" s="7">
         <f>'Initial Buys'!Z40</f>
         <v>1093.28</v>
       </c>
-      <c r="G10" s="26">
+      <c r="G13" s="27">
         <f>'2016'!S10</f>
         <v>5.97</v>
       </c>
-      <c r="H10" s="24">
-        <v>0</v>
-      </c>
-      <c r="I10" s="21">
-        <v>0</v>
-      </c>
-      <c r="J10" s="24">
+      <c r="H13" s="24">
+        <v>0</v>
+      </c>
+      <c r="I13" s="21">
+        <v>0</v>
+      </c>
+      <c r="J13" s="24">
         <v>6.04</v>
       </c>
-      <c r="K10" s="21">
-        <v>0</v>
-      </c>
-      <c r="L10" s="24">
-        <v>0</v>
-      </c>
-      <c r="M10" s="21">
+      <c r="K13" s="21">
+        <v>0</v>
+      </c>
+      <c r="L13" s="24">
+        <v>0</v>
+      </c>
+      <c r="M13" s="21">
         <v>6.07</v>
       </c>
-      <c r="N10" s="24">
-        <v>0</v>
-      </c>
-      <c r="O10" s="21">
-        <v>0</v>
-      </c>
-      <c r="P10" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="21">
-        <v>0</v>
-      </c>
-      <c r="R10" s="24">
-        <v>0</v>
-      </c>
-      <c r="S10" s="21">
-        <v>0</v>
-      </c>
-      <c r="T10" s="17">
+      <c r="N13" s="24">
+        <v>0</v>
+      </c>
+      <c r="O13" s="21">
+        <v>0</v>
+      </c>
+      <c r="P13" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="21">
+        <v>0</v>
+      </c>
+      <c r="R13" s="24">
+        <v>0</v>
+      </c>
+      <c r="S13" s="21">
+        <v>0</v>
+      </c>
+      <c r="T13" s="18">
         <f t="shared" si="2"/>
         <v>12.11</v>
       </c>
-      <c r="U10" s="17">
+      <c r="U13" s="18">
         <f t="shared" si="3"/>
         <v>18.079999999999998</v>
       </c>
-      <c r="V10" s="15">
+      <c r="V13" s="16">
         <f t="shared" si="1"/>
         <v>1111.3599999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="8">
+        <v>20</v>
+      </c>
+      <c r="E14" s="33">
+        <f t="shared" si="0"/>
+        <v>49.97</v>
+      </c>
+      <c r="F14" s="9">
+        <f>'Initial Buys'!I83</f>
+        <v>999.4</v>
+      </c>
+      <c r="G14" s="32">
+        <v>0</v>
+      </c>
+      <c r="H14" s="24">
+        <v>0</v>
+      </c>
+      <c r="I14" s="21">
+        <v>0</v>
+      </c>
+      <c r="J14" s="24">
+        <v>0</v>
+      </c>
+      <c r="K14" s="21">
+        <v>0</v>
+      </c>
+      <c r="L14" s="24">
+        <v>0</v>
+      </c>
+      <c r="M14" s="21">
+        <v>0</v>
+      </c>
+      <c r="N14" s="24">
+        <v>0</v>
+      </c>
+      <c r="O14" s="21">
+        <v>0</v>
+      </c>
+      <c r="P14" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="21">
+        <v>0</v>
+      </c>
+      <c r="R14" s="24">
+        <v>0</v>
+      </c>
+      <c r="S14" s="21">
+        <v>0</v>
+      </c>
+      <c r="T14" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U14" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V14" s="15">
+        <f t="shared" si="1"/>
+        <v>999.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C15" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D15" s="6">
         <v>34.256</v>
       </c>
-      <c r="E11" s="34">
-        <f>V11/D11</f>
+      <c r="E15" s="34">
+        <f>V15/D15</f>
         <v>39.889946286781871</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F15" s="7">
         <f>'Initial Buys'!AF40</f>
         <v>1356.1799999999998</v>
       </c>
-      <c r="G11" s="27">
-        <v>0</v>
-      </c>
-      <c r="H11" s="24">
-        <v>0</v>
-      </c>
-      <c r="I11" s="21">
-        <v>0</v>
-      </c>
-      <c r="J11" s="24">
-        <v>0</v>
-      </c>
-      <c r="K11" s="21">
-        <v>0</v>
-      </c>
-      <c r="L11" s="24">
+      <c r="G15" s="27">
+        <v>0</v>
+      </c>
+      <c r="H15" s="24">
+        <v>0</v>
+      </c>
+      <c r="I15" s="21">
+        <v>0</v>
+      </c>
+      <c r="J15" s="24">
+        <v>0</v>
+      </c>
+      <c r="K15" s="21">
+        <v>0</v>
+      </c>
+      <c r="L15" s="24">
         <v>10.29</v>
       </c>
-      <c r="M11" s="21">
-        <v>0</v>
-      </c>
-      <c r="N11" s="24">
-        <v>0</v>
-      </c>
-      <c r="O11" s="21">
-        <v>0</v>
-      </c>
-      <c r="P11" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="21">
-        <v>0</v>
-      </c>
-      <c r="R11" s="24">
-        <v>0</v>
-      </c>
-      <c r="S11" s="21">
-        <v>0</v>
-      </c>
-      <c r="T11" s="18">
-        <f>SUM(H11:S11)</f>
+      <c r="M15" s="21">
+        <v>0</v>
+      </c>
+      <c r="N15" s="24">
+        <v>0</v>
+      </c>
+      <c r="O15" s="21">
+        <v>0</v>
+      </c>
+      <c r="P15" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="21">
+        <v>0</v>
+      </c>
+      <c r="R15" s="24">
+        <v>0</v>
+      </c>
+      <c r="S15" s="21">
+        <v>0</v>
+      </c>
+      <c r="T15" s="18">
+        <f>SUM(H15:S15)</f>
         <v>10.29</v>
       </c>
-      <c r="U11" s="18">
-        <f>SUM(G11:S11)</f>
+      <c r="U15" s="18">
+        <f>SUM(G15:S15)</f>
         <v>10.29</v>
       </c>
-      <c r="V11" s="16">
-        <f>SUM(F11, U11)</f>
+      <c r="V15" s="16">
+        <f>SUM(F15, U15)</f>
         <v>1366.4699999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C16" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D16" s="8">
         <v>15.423999999999999</v>
       </c>
-      <c r="E12" s="33">
-        <f>V12/D12</f>
+      <c r="E16" s="33">
+        <f>V16/D16</f>
         <v>71.919087136929477</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F16" s="9">
         <f>'Initial Buys'!AC40</f>
         <v>1078.6500000000001</v>
       </c>
-      <c r="G12" s="32">
+      <c r="G16" s="32">
         <f>'2016'!S11</f>
         <v>7.5</v>
       </c>
-      <c r="H12" s="24">
+      <c r="H16" s="24">
         <v>7.55</v>
       </c>
-      <c r="I12" s="21">
-        <v>0</v>
-      </c>
-      <c r="J12" s="24">
-        <v>0</v>
-      </c>
-      <c r="K12" s="21">
+      <c r="I16" s="21">
+        <v>0</v>
+      </c>
+      <c r="J16" s="24">
+        <v>0</v>
+      </c>
+      <c r="K16" s="21">
         <v>7.76</v>
       </c>
-      <c r="L12" s="24">
-        <v>0</v>
-      </c>
-      <c r="M12" s="21">
+      <c r="L16" s="24">
+        <v>0</v>
+      </c>
+      <c r="M16" s="21">
         <v>7.82</v>
       </c>
-      <c r="N12" s="24">
-        <v>0</v>
-      </c>
-      <c r="O12" s="21">
-        <v>0</v>
-      </c>
-      <c r="P12" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="21">
-        <v>0</v>
-      </c>
-      <c r="R12" s="24">
-        <v>0</v>
-      </c>
-      <c r="S12" s="21">
-        <v>0</v>
-      </c>
-      <c r="T12" s="17">
-        <f>SUM(H12:S12)</f>
+      <c r="N16" s="24">
+        <v>0</v>
+      </c>
+      <c r="O16" s="21">
+        <v>0</v>
+      </c>
+      <c r="P16" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="21">
+        <v>0</v>
+      </c>
+      <c r="R16" s="24">
+        <v>0</v>
+      </c>
+      <c r="S16" s="21">
+        <v>0</v>
+      </c>
+      <c r="T16" s="17">
+        <f>SUM(H16:S16)</f>
         <v>23.13</v>
       </c>
-      <c r="U12" s="17">
-        <f>SUM(G12:S12)</f>
+      <c r="U16" s="17">
+        <f>SUM(G16:S16)</f>
         <v>30.630000000000003</v>
       </c>
-      <c r="V12" s="15">
-        <f>SUM(F12, U12)</f>
+      <c r="V16" s="15">
+        <f>SUM(F16, U16)</f>
         <v>1109.2800000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B17" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C17" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D17" s="6">
         <v>12.224</v>
       </c>
-      <c r="E13" s="34">
-        <f t="shared" ref="E13" si="4">V13/D13</f>
+      <c r="E17" s="34">
+        <f t="shared" ref="E17" si="4">V17/D17</f>
         <v>86.796465968586389</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F17" s="7">
         <f>'Initial Buys'!B83</f>
         <v>1042.68</v>
       </c>
-      <c r="G13" s="27">
-        <v>0</v>
-      </c>
-      <c r="H13" s="24">
-        <v>0</v>
-      </c>
-      <c r="I13" s="21">
-        <v>0</v>
-      </c>
-      <c r="J13" s="24">
+      <c r="G17" s="27">
+        <v>0</v>
+      </c>
+      <c r="H17" s="24">
+        <v>0</v>
+      </c>
+      <c r="I17" s="21">
+        <v>0</v>
+      </c>
+      <c r="J17" s="24">
         <v>9</v>
       </c>
-      <c r="K13" s="21">
-        <v>0</v>
-      </c>
-      <c r="L13" s="24">
-        <v>0</v>
-      </c>
-      <c r="M13" s="21">
+      <c r="K17" s="21">
+        <v>0</v>
+      </c>
+      <c r="L17" s="24">
+        <v>0</v>
+      </c>
+      <c r="M17" s="21">
         <v>9.32</v>
       </c>
-      <c r="N13" s="24">
-        <v>0</v>
-      </c>
-      <c r="O13" s="21">
-        <v>0</v>
-      </c>
-      <c r="P13" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="21">
-        <v>0</v>
-      </c>
-      <c r="R13" s="24">
-        <v>0</v>
-      </c>
-      <c r="S13" s="21">
-        <v>0</v>
-      </c>
-      <c r="T13" s="18">
-        <f t="shared" ref="T13" si="5">SUM(H13:S13)</f>
+      <c r="N17" s="24">
+        <v>0</v>
+      </c>
+      <c r="O17" s="21">
+        <v>0</v>
+      </c>
+      <c r="P17" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="21">
+        <v>0</v>
+      </c>
+      <c r="R17" s="24">
+        <v>0</v>
+      </c>
+      <c r="S17" s="21">
+        <v>0</v>
+      </c>
+      <c r="T17" s="18">
+        <f t="shared" ref="T17" si="5">SUM(H17:S17)</f>
         <v>18.32</v>
       </c>
-      <c r="U13" s="18">
-        <f t="shared" ref="U13" si="6">SUM(G13:S13)</f>
+      <c r="U17" s="18">
+        <f t="shared" ref="U17" si="6">SUM(G17:S17)</f>
         <v>18.32</v>
       </c>
-      <c r="V13" s="16">
-        <f t="shared" ref="V13" si="7">SUM(F13, U13)</f>
+      <c r="V17" s="16">
+        <f t="shared" ref="V17" si="7">SUM(F17, U17)</f>
         <v>1061</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="29">
-        <f t="shared" ref="F14:V14" si="8">SUM(F2:F13)</f>
-        <v>12810.330000000002</v>
-      </c>
-      <c r="G14" s="30">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="28"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="29">
+        <f t="shared" ref="F18:V18" si="8">SUM(F2:F17)</f>
+        <v>16781.767</v>
+      </c>
+      <c r="G18" s="30">
         <f t="shared" si="8"/>
         <v>89.969999999999985</v>
       </c>
-      <c r="H14" s="31">
+      <c r="H18" s="31">
         <f t="shared" si="8"/>
         <v>12.74</v>
       </c>
-      <c r="I14" s="30">
+      <c r="I18" s="30">
         <f t="shared" si="8"/>
         <v>9.74</v>
       </c>
-      <c r="J14" s="31">
+      <c r="J18" s="31">
         <f t="shared" si="8"/>
         <v>49.989999999999995</v>
       </c>
-      <c r="K14" s="30">
+      <c r="K18" s="30">
         <f t="shared" si="8"/>
         <v>12.98</v>
       </c>
-      <c r="L14" s="31">
+      <c r="L18" s="31">
         <f t="shared" si="8"/>
         <v>20.079999999999998</v>
       </c>
-      <c r="M14" s="30">
+      <c r="M18" s="30">
         <f t="shared" si="8"/>
         <v>58.75</v>
       </c>
-      <c r="N14" s="31">
+      <c r="N18" s="31">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="O14" s="30">
+      <c r="O18" s="30">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P14" s="31">
+      <c r="P18" s="31">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Q14" s="30">
+      <c r="Q18" s="30">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="R14" s="31">
+      <c r="R18" s="31">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S14" s="30">
+      <c r="S18" s="30">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="T14" s="30">
+      <c r="T18" s="30">
         <f t="shared" si="8"/>
         <v>164.27999999999997</v>
       </c>
-      <c r="U14" s="30">
+      <c r="U18" s="30">
         <f t="shared" si="8"/>
         <v>254.24999999999997</v>
       </c>
-      <c r="V14" s="23">
+      <c r="V18" s="23">
         <f t="shared" si="8"/>
-        <v>13064.580000000002</v>
+        <v>17036.017</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated 401k, ira, and total dividend excel sheets.
</commit_message>
<xml_diff>
--- a/DividendLiberty/401k.xlsx
+++ b/DividendLiberty/401k.xlsx
@@ -680,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF83"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="R83" sqref="R83"/>
+    <sheetView topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,7 +874,12 @@
       <c r="Q3" s="5"/>
       <c r="T3" s="5"/>
       <c r="W3" s="5"/>
-      <c r="Z3" s="19"/>
+      <c r="Y3" s="4">
+        <v>42985</v>
+      </c>
+      <c r="Z3" s="19">
+        <v>316.89</v>
+      </c>
       <c r="AE3" s="4">
         <v>42902</v>
       </c>
@@ -891,7 +896,12 @@
       <c r="Q4" s="5"/>
       <c r="T4" s="5"/>
       <c r="W4" s="5"/>
-      <c r="Z4" s="5"/>
+      <c r="Y4" s="4">
+        <v>42985</v>
+      </c>
+      <c r="Z4" s="5">
+        <v>634.55999999999995</v>
+      </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
@@ -1314,7 +1324,7 @@
       </c>
       <c r="Z40" s="19">
         <f>SUM(Z2:Z39)</f>
-        <v>1093.28</v>
+        <v>2044.73</v>
       </c>
       <c r="AC40" s="19">
         <f>SUM(AC2:AC39)</f>
@@ -2370,11 +2380,11 @@
         <v>7</v>
       </c>
       <c r="D2" s="8">
-        <v>22.254000000000001</v>
+        <v>22.338999999999999</v>
       </c>
       <c r="E2" s="33">
         <f t="shared" ref="E2:E15" si="0">V2/D2</f>
-        <v>47.214433360294777</v>
+        <v>47.224137159228263</v>
       </c>
       <c r="F2" s="9">
         <f>'Initial Buys'!B40</f>
@@ -2409,7 +2419,7 @@
         <v>0</v>
       </c>
       <c r="P2" s="24">
-        <v>0</v>
+        <v>4.2300000000000004</v>
       </c>
       <c r="Q2" s="21">
         <v>0</v>
@@ -2422,15 +2432,15 @@
       </c>
       <c r="T2" s="17">
         <f>SUM(H2:S2)</f>
-        <v>8.41</v>
+        <v>12.64</v>
       </c>
       <c r="U2" s="17">
         <f>SUM(G2:S2)</f>
-        <v>12.309999999999999</v>
+        <v>16.54</v>
       </c>
       <c r="V2" s="15">
         <f t="shared" ref="V2:V15" si="1">SUM(F2, U2)</f>
-        <v>1050.71</v>
+        <v>1054.94</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -3254,15 +3264,15 @@
         <v>7</v>
       </c>
       <c r="D14" s="8">
-        <v>8.1370000000000005</v>
+        <v>17.196999999999999</v>
       </c>
       <c r="E14" s="33">
         <f t="shared" si="0"/>
-        <v>136.58104952685264</v>
+        <v>120.32098621852649</v>
       </c>
       <c r="F14" s="9">
         <f>'Initial Buys'!Z40</f>
-        <v>1093.28</v>
+        <v>2044.73</v>
       </c>
       <c r="G14" s="32">
         <f>'2016'!S10</f>
@@ -3293,7 +3303,7 @@
         <v>0</v>
       </c>
       <c r="P14" s="24">
-        <v>0</v>
+        <v>6.35</v>
       </c>
       <c r="Q14" s="21">
         <v>0</v>
@@ -3306,15 +3316,15 @@
       </c>
       <c r="T14" s="17">
         <f t="shared" si="2"/>
-        <v>12.11</v>
+        <v>18.46</v>
       </c>
       <c r="U14" s="17">
         <f t="shared" si="3"/>
-        <v>18.079999999999998</v>
+        <v>24.43</v>
       </c>
       <c r="V14" s="15">
         <f t="shared" si="1"/>
-        <v>1111.3599999999999</v>
+        <v>2069.16</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
@@ -3328,11 +3338,11 @@
         <v>62</v>
       </c>
       <c r="D15" s="6">
-        <v>20</v>
+        <v>20.239999999999998</v>
       </c>
       <c r="E15" s="34">
         <f t="shared" si="0"/>
-        <v>49.97</v>
+        <v>49.950592885375499</v>
       </c>
       <c r="F15" s="7">
         <f>'Initial Buys'!I83</f>
@@ -3366,7 +3376,7 @@
         <v>0</v>
       </c>
       <c r="P15" s="24">
-        <v>0</v>
+        <v>11.6</v>
       </c>
       <c r="Q15" s="21">
         <v>0</v>
@@ -3379,15 +3389,15 @@
       </c>
       <c r="T15" s="18">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>11.6</v>
       </c>
       <c r="U15" s="18">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>11.6</v>
       </c>
       <c r="V15" s="16">
         <f t="shared" si="1"/>
-        <v>999.4</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
@@ -3474,11 +3484,11 @@
         <v>7</v>
       </c>
       <c r="D17" s="6">
-        <v>15.423999999999999</v>
+        <v>15.523999999999999</v>
       </c>
       <c r="E17" s="34">
         <f>V17/D17</f>
-        <v>71.919087136929477</v>
+        <v>71.962767328008255</v>
       </c>
       <c r="F17" s="7">
         <f>'Initial Buys'!AC40</f>
@@ -3513,7 +3523,7 @@
         <v>0</v>
       </c>
       <c r="P17" s="24">
-        <v>0</v>
+        <v>7.87</v>
       </c>
       <c r="Q17" s="21">
         <v>0</v>
@@ -3526,15 +3536,15 @@
       </c>
       <c r="T17" s="18">
         <f>SUM(H17:S17)</f>
-        <v>23.13</v>
+        <v>31</v>
       </c>
       <c r="U17" s="18">
         <f>SUM(G17:S17)</f>
-        <v>30.630000000000003</v>
+        <v>38.5</v>
       </c>
       <c r="V17" s="16">
         <f>SUM(F17, U17)</f>
-        <v>1109.2800000000002</v>
+        <v>1117.1500000000001</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
@@ -3618,7 +3628,7 @@
       <c r="E19" s="28"/>
       <c r="F19" s="29">
         <f t="shared" ref="F19:V19" si="11">SUM(F2:F18)</f>
-        <v>17977.687000000002</v>
+        <v>18929.136999999999</v>
       </c>
       <c r="G19" s="30">
         <f t="shared" si="11"/>
@@ -3658,7 +3668,7 @@
       </c>
       <c r="P19" s="31">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>30.05</v>
       </c>
       <c r="Q19" s="30">
         <f t="shared" si="11"/>
@@ -3674,15 +3684,15 @@
       </c>
       <c r="T19" s="30">
         <f t="shared" si="11"/>
-        <v>205.89999999999998</v>
+        <v>235.95</v>
       </c>
       <c r="U19" s="30">
         <f t="shared" si="11"/>
-        <v>295.86999999999995</v>
+        <v>325.91999999999996</v>
       </c>
       <c r="V19" s="23">
         <f t="shared" si="11"/>
-        <v>18273.557000000001</v>
+        <v>19255.057000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated excel files and added mortgage.
</commit_message>
<xml_diff>
--- a/DividendLiberty/401k.xlsx
+++ b/DividendLiberty/401k.xlsx
@@ -2287,7 +2287,7 @@
   <dimension ref="A1:V19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3499,11 +3499,11 @@
         <v>7</v>
       </c>
       <c r="D17" s="6">
-        <v>15.523999999999999</v>
+        <v>15.603999999999999</v>
       </c>
       <c r="E17" s="34">
         <f>V17/D17</f>
-        <v>71.962767328008255</v>
+        <v>72.101384260446054</v>
       </c>
       <c r="F17" s="7">
         <f>'Initial Buys'!AC40</f>
@@ -3547,19 +3547,19 @@
         <v>0</v>
       </c>
       <c r="S17" s="21">
-        <v>0</v>
+        <v>7.92</v>
       </c>
       <c r="T17" s="18">
         <f>SUM(H17:S17)</f>
-        <v>31</v>
+        <v>38.92</v>
       </c>
       <c r="U17" s="18">
         <f>SUM(G17:S17)</f>
-        <v>38.5</v>
+        <v>46.42</v>
       </c>
       <c r="V17" s="16">
         <f>SUM(F17, U17)</f>
-        <v>1117.1500000000001</v>
+        <v>1125.0700000000002</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
@@ -3695,19 +3695,19 @@
       </c>
       <c r="S19" s="30">
         <f t="shared" si="11"/>
-        <v>97.439999999999984</v>
+        <v>105.35999999999999</v>
       </c>
       <c r="T19" s="30">
         <f t="shared" si="11"/>
-        <v>424.82</v>
+        <v>432.74</v>
       </c>
       <c r="U19" s="30">
         <f t="shared" si="11"/>
-        <v>514.79000000000008</v>
+        <v>522.71</v>
       </c>
       <c r="V19" s="23">
         <f t="shared" si="11"/>
-        <v>21931.377000000004</v>
+        <v>21939.297000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated dividends and added traditional ira.
</commit_message>
<xml_diff>
--- a/DividendLiberty/401k.xlsx
+++ b/DividendLiberty/401k.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Initial Buys" sheetId="3" r:id="rId1"/>
     <sheet name="2016" sheetId="2" r:id="rId2"/>
     <sheet name="2017" sheetId="4" r:id="rId3"/>
+    <sheet name="2018" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="66">
   <si>
     <t>Symbols</t>
   </si>
@@ -2286,8 +2287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2402,7 +2403,6 @@
         <v>47.422268183385036</v>
       </c>
       <c r="F2" s="9">
-        <f>'Initial Buys'!B40</f>
         <v>2038.81</v>
       </c>
       <c r="G2" s="26">
@@ -2476,7 +2476,6 @@
         <v>135.90252707581229</v>
       </c>
       <c r="F3" s="7">
-        <f>'Initial Buys'!E40</f>
         <v>1089.68</v>
       </c>
       <c r="G3" s="27">
@@ -2550,7 +2549,6 @@
         <v>105.20847121111845</v>
       </c>
       <c r="F4" s="9">
-        <f>'Initial Buys'!F83</f>
         <v>946.8</v>
       </c>
       <c r="G4" s="32">
@@ -2623,7 +2621,6 @@
         <v>50.407104085325201</v>
       </c>
       <c r="F5" s="7">
-        <f>'Initial Buys'!H40</f>
         <v>999.8</v>
       </c>
       <c r="G5" s="27">
@@ -2694,11 +2691,10 @@
       </c>
       <c r="E6" s="33">
         <f t="shared" si="0"/>
-        <v>33.877312441035322</v>
+        <v>33.877312441035315</v>
       </c>
       <c r="F6" s="9">
-        <f>'Initial Buys'!K40</f>
-        <v>1625.8200000000002</v>
+        <v>1625.82</v>
       </c>
       <c r="G6" s="32">
         <f>'2016'!S5</f>
@@ -2750,7 +2746,7 @@
       </c>
       <c r="V6" s="15">
         <f t="shared" si="1"/>
-        <v>1651.7900000000002</v>
+        <v>1651.79</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -2771,7 +2767,6 @@
         <v>36.289190735776884</v>
       </c>
       <c r="F7" s="7">
-        <f>'Initial Buys'!R83</f>
         <v>1195.92</v>
       </c>
       <c r="G7" s="27">
@@ -2844,7 +2839,6 @@
         <v>119.08731431014215</v>
       </c>
       <c r="F8" s="9">
-        <f>'Initial Buys'!N40</f>
         <v>1069.29</v>
       </c>
       <c r="G8" s="32">
@@ -2918,7 +2912,6 @@
         <v>82.335393138717237</v>
       </c>
       <c r="F9" s="7">
-        <f>'Initial Buys'!Q40</f>
         <v>1892.99</v>
       </c>
       <c r="G9" s="27">
@@ -2992,7 +2985,6 @@
         <v>119.31108977436389</v>
       </c>
       <c r="F10" s="9">
-        <f>'Initial Buys'!T40</f>
         <v>948</v>
       </c>
       <c r="G10" s="32">
@@ -3066,7 +3058,6 @@
         <v>96.142857142857139</v>
       </c>
       <c r="F11" s="7">
-        <f>'Initial Buys'!W40</f>
         <v>1062.5999999999999</v>
       </c>
       <c r="G11" s="27">
@@ -3140,7 +3131,6 @@
         <v>213.04724214692058</v>
       </c>
       <c r="F12" s="9">
-        <f>'Initial Buys'!L83</f>
         <v>851.92</v>
       </c>
       <c r="G12" s="32">
@@ -3210,11 +3200,10 @@
       </c>
       <c r="E13" s="34">
         <f t="shared" si="0"/>
-        <v>117.28055197061451</v>
+        <v>117.28084979648564</v>
       </c>
       <c r="F13" s="7">
-        <f>'Initial Buys'!O83</f>
-        <v>1173.317</v>
+        <v>1173.32</v>
       </c>
       <c r="G13" s="27">
         <v>0</v>
@@ -3265,7 +3254,7 @@
       </c>
       <c r="V13" s="16">
         <f t="shared" si="1"/>
-        <v>1181.367</v>
+        <v>1181.3699999999999</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -3286,7 +3275,6 @@
         <v>120.30327537403964</v>
       </c>
       <c r="F14" s="9">
-        <f>'Initial Buys'!Z40</f>
         <v>2044.73</v>
       </c>
       <c r="G14" s="32">
@@ -3360,7 +3348,6 @@
         <v>49.960431830394214</v>
       </c>
       <c r="F15" s="7">
-        <f>'Initial Buys'!I83</f>
         <v>999.4</v>
       </c>
       <c r="G15" s="27">
@@ -3430,11 +3417,10 @@
       </c>
       <c r="E16" s="33">
         <f>V16/D16</f>
-        <v>39.793679663521644</v>
+        <v>39.793679663521651</v>
       </c>
       <c r="F16" s="9">
-        <f>'Initial Buys'!AF40</f>
-        <v>1356.1799999999998</v>
+        <v>1356.18</v>
       </c>
       <c r="G16" s="32">
         <v>0</v>
@@ -3485,7 +3471,7 @@
       </c>
       <c r="V16" s="15">
         <f>SUM(F16, U16)</f>
-        <v>1400.2599999999998</v>
+        <v>1400.26</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
@@ -3499,14 +3485,13 @@
         <v>7</v>
       </c>
       <c r="D17" s="6">
-        <v>15.603999999999999</v>
+        <v>15.523999999999999</v>
       </c>
       <c r="E17" s="34">
         <f>V17/D17</f>
-        <v>72.101384260446054</v>
+        <v>71.962767328008255</v>
       </c>
       <c r="F17" s="7">
-        <f>'Initial Buys'!AC40</f>
         <v>1078.6500000000001</v>
       </c>
       <c r="G17" s="27">
@@ -3547,19 +3532,19 @@
         <v>0</v>
       </c>
       <c r="S17" s="21">
-        <v>7.92</v>
+        <v>0</v>
       </c>
       <c r="T17" s="18">
         <f>SUM(H17:S17)</f>
-        <v>38.92</v>
+        <v>31</v>
       </c>
       <c r="U17" s="18">
         <f>SUM(G17:S17)</f>
-        <v>46.42</v>
+        <v>38.5</v>
       </c>
       <c r="V17" s="16">
         <f>SUM(F17, U17)</f>
-        <v>1125.0700000000002</v>
+        <v>1117.1500000000001</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
@@ -3580,7 +3565,6 @@
         <v>86.684058436346135</v>
       </c>
       <c r="F18" s="9">
-        <f>'Initial Buys'!B83</f>
         <v>1042.68</v>
       </c>
       <c r="G18" s="32">
@@ -3643,7 +3627,7 @@
       <c r="E19" s="28"/>
       <c r="F19" s="29">
         <f t="shared" ref="F19:V19" si="11">SUM(F2:F18)</f>
-        <v>21416.587000000003</v>
+        <v>21416.590000000004</v>
       </c>
       <c r="G19" s="30">
         <f t="shared" si="11"/>
@@ -3695,23 +3679,1452 @@
       </c>
       <c r="S19" s="30">
         <f t="shared" si="11"/>
-        <v>105.35999999999999</v>
+        <v>97.439999999999984</v>
       </c>
       <c r="T19" s="30">
         <f t="shared" si="11"/>
-        <v>432.74</v>
+        <v>424.82</v>
       </c>
       <c r="U19" s="30">
         <f t="shared" si="11"/>
-        <v>522.71</v>
+        <v>514.79000000000008</v>
       </c>
       <c r="V19" s="23">
         <f t="shared" si="11"/>
-        <v>21939.297000000002</v>
+        <v>21931.38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="U1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="V1" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="8">
+        <v>43.515000000000001</v>
+      </c>
+      <c r="E2" s="33">
+        <f t="shared" ref="E2:E15" si="0">V2/D2</f>
+        <v>47.422268183385036</v>
+      </c>
+      <c r="F2" s="9">
+        <f>'Initial Buys'!B40</f>
+        <v>2038.81</v>
+      </c>
+      <c r="G2" s="26">
+        <f>'2017'!U2</f>
+        <v>24.77</v>
+      </c>
+      <c r="H2" s="24">
+        <v>0</v>
+      </c>
+      <c r="I2" s="21">
+        <v>0</v>
+      </c>
+      <c r="J2" s="24">
+        <v>0</v>
+      </c>
+      <c r="K2" s="21">
+        <v>0</v>
+      </c>
+      <c r="L2" s="24">
+        <v>0</v>
+      </c>
+      <c r="M2" s="21">
+        <v>0</v>
+      </c>
+      <c r="N2" s="24">
+        <v>0</v>
+      </c>
+      <c r="O2" s="21">
+        <v>0</v>
+      </c>
+      <c r="P2" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="21">
+        <v>0</v>
+      </c>
+      <c r="R2" s="24">
+        <v>0</v>
+      </c>
+      <c r="S2" s="21">
+        <v>0</v>
+      </c>
+      <c r="T2" s="17">
+        <f>SUM(H2:S2)</f>
+        <v>0</v>
+      </c>
+      <c r="U2" s="17">
+        <f>SUM(G2:S2)</f>
+        <v>24.77</v>
+      </c>
+      <c r="V2" s="15">
+        <f t="shared" ref="V2:V15" si="1">SUM(F2, U2)</f>
+        <v>2063.58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="6">
+        <v>8.31</v>
+      </c>
+      <c r="E3" s="34">
+        <f t="shared" si="0"/>
+        <v>135.90252707581229</v>
+      </c>
+      <c r="F3" s="7">
+        <f>'Initial Buys'!E40</f>
+        <v>1089.68</v>
+      </c>
+      <c r="G3" s="27">
+        <f>'2017'!U3</f>
+        <v>39.669999999999995</v>
+      </c>
+      <c r="H3" s="24">
+        <v>0</v>
+      </c>
+      <c r="I3" s="21">
+        <v>0</v>
+      </c>
+      <c r="J3" s="24">
+        <v>0</v>
+      </c>
+      <c r="K3" s="21">
+        <v>0</v>
+      </c>
+      <c r="L3" s="24">
+        <v>0</v>
+      </c>
+      <c r="M3" s="21">
+        <v>0</v>
+      </c>
+      <c r="N3" s="24">
+        <v>0</v>
+      </c>
+      <c r="O3" s="21">
+        <v>0</v>
+      </c>
+      <c r="P3" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="21">
+        <v>0</v>
+      </c>
+      <c r="R3" s="24">
+        <v>0</v>
+      </c>
+      <c r="S3" s="21">
+        <v>0</v>
+      </c>
+      <c r="T3" s="18">
+        <f t="shared" ref="T3:T15" si="2">SUM(H3:S3)</f>
+        <v>0</v>
+      </c>
+      <c r="U3" s="18">
+        <f t="shared" ref="U3:U15" si="3">SUM(G3:S3)</f>
+        <v>39.669999999999995</v>
+      </c>
+      <c r="V3" s="16">
+        <f>SUM(F3, U3)</f>
+        <v>1129.3500000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="8">
+        <v>9.0660000000000007</v>
+      </c>
+      <c r="E4" s="33">
+        <f t="shared" si="0"/>
+        <v>105.20847121111845</v>
+      </c>
+      <c r="F4" s="9">
+        <f>'Initial Buys'!F83</f>
+        <v>946.8</v>
+      </c>
+      <c r="G4" s="32">
+        <f>'2017'!U4</f>
+        <v>7.02</v>
+      </c>
+      <c r="H4" s="24">
+        <v>0</v>
+      </c>
+      <c r="I4" s="21">
+        <v>0</v>
+      </c>
+      <c r="J4" s="24">
+        <v>0</v>
+      </c>
+      <c r="K4" s="21">
+        <v>0</v>
+      </c>
+      <c r="L4" s="24">
+        <v>0</v>
+      </c>
+      <c r="M4" s="21">
+        <v>0</v>
+      </c>
+      <c r="N4" s="24">
+        <v>0</v>
+      </c>
+      <c r="O4" s="21">
+        <v>0</v>
+      </c>
+      <c r="P4" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="21">
+        <v>0</v>
+      </c>
+      <c r="R4" s="24">
+        <v>0</v>
+      </c>
+      <c r="S4" s="21">
+        <v>0</v>
+      </c>
+      <c r="T4" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U4" s="17">
+        <f t="shared" si="3"/>
+        <v>7.02</v>
+      </c>
+      <c r="V4" s="15">
+        <f>SUM(F4, U4)</f>
+        <v>953.81999999999994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="6">
+        <v>21.001999999999999</v>
+      </c>
+      <c r="E5" s="34">
+        <f t="shared" si="0"/>
+        <v>50.407104085325201</v>
+      </c>
+      <c r="F5" s="7">
+        <f>'Initial Buys'!H40</f>
+        <v>999.8</v>
+      </c>
+      <c r="G5" s="27">
+        <f>'2017'!U5</f>
+        <v>58.849999999999994</v>
+      </c>
+      <c r="H5" s="24">
+        <v>0</v>
+      </c>
+      <c r="I5" s="21">
+        <v>0</v>
+      </c>
+      <c r="J5" s="24">
+        <v>0</v>
+      </c>
+      <c r="K5" s="21">
+        <v>0</v>
+      </c>
+      <c r="L5" s="24">
+        <v>0</v>
+      </c>
+      <c r="M5" s="21">
+        <v>0</v>
+      </c>
+      <c r="N5" s="24">
+        <v>0</v>
+      </c>
+      <c r="O5" s="21">
+        <v>0</v>
+      </c>
+      <c r="P5" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="21">
+        <v>0</v>
+      </c>
+      <c r="R5" s="24">
+        <v>0</v>
+      </c>
+      <c r="S5" s="21">
+        <v>0</v>
+      </c>
+      <c r="T5" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U5" s="18">
+        <f t="shared" si="3"/>
+        <v>58.849999999999994</v>
+      </c>
+      <c r="V5" s="16">
+        <f t="shared" si="1"/>
+        <v>1058.6499999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="8">
+        <v>48.758000000000003</v>
+      </c>
+      <c r="E6" s="33">
+        <f t="shared" si="0"/>
+        <v>33.877312441035322</v>
+      </c>
+      <c r="F6" s="9">
+        <f>'Initial Buys'!K40</f>
+        <v>1625.8200000000002</v>
+      </c>
+      <c r="G6" s="32">
+        <f>'2017'!U6</f>
+        <v>25.97</v>
+      </c>
+      <c r="H6" s="24">
+        <v>0</v>
+      </c>
+      <c r="I6" s="21">
+        <v>0</v>
+      </c>
+      <c r="J6" s="24">
+        <v>0</v>
+      </c>
+      <c r="K6" s="21">
+        <v>0</v>
+      </c>
+      <c r="L6" s="24">
+        <v>0</v>
+      </c>
+      <c r="M6" s="21">
+        <v>0</v>
+      </c>
+      <c r="N6" s="24">
+        <v>0</v>
+      </c>
+      <c r="O6" s="21">
+        <v>0</v>
+      </c>
+      <c r="P6" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="21">
+        <v>0</v>
+      </c>
+      <c r="R6" s="24">
+        <v>0</v>
+      </c>
+      <c r="S6" s="21">
+        <v>0</v>
+      </c>
+      <c r="T6" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U6" s="17">
+        <f t="shared" si="3"/>
+        <v>25.97</v>
+      </c>
+      <c r="V6" s="15">
+        <f t="shared" si="1"/>
+        <v>1651.7900000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="6">
+        <v>33.203000000000003</v>
+      </c>
+      <c r="E7" s="34">
+        <f t="shared" si="0"/>
+        <v>36.289190735776884</v>
+      </c>
+      <c r="F7" s="7">
+        <f>'Initial Buys'!R83</f>
+        <v>1195.92</v>
+      </c>
+      <c r="G7" s="27">
+        <f>'2017'!U7</f>
+        <v>8.99</v>
+      </c>
+      <c r="H7" s="24">
+        <v>0</v>
+      </c>
+      <c r="I7" s="21">
+        <v>0</v>
+      </c>
+      <c r="J7" s="24">
+        <v>0</v>
+      </c>
+      <c r="K7" s="21">
+        <v>0</v>
+      </c>
+      <c r="L7" s="24">
+        <v>0</v>
+      </c>
+      <c r="M7" s="21">
+        <v>0</v>
+      </c>
+      <c r="N7" s="24">
+        <v>0</v>
+      </c>
+      <c r="O7" s="21">
+        <v>0</v>
+      </c>
+      <c r="P7" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="21">
+        <v>0</v>
+      </c>
+      <c r="R7" s="24">
+        <v>0</v>
+      </c>
+      <c r="S7" s="21">
+        <v>0</v>
+      </c>
+      <c r="T7" s="18">
+        <f t="shared" ref="T7" si="4">SUM(H7:S7)</f>
+        <v>0</v>
+      </c>
+      <c r="U7" s="18">
+        <f t="shared" ref="U7" si="5">SUM(G7:S7)</f>
+        <v>8.99</v>
+      </c>
+      <c r="V7" s="16">
+        <f t="shared" si="1"/>
+        <v>1204.9100000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="8">
+        <v>9.3569999999999993</v>
+      </c>
+      <c r="E8" s="33">
+        <f t="shared" si="0"/>
+        <v>119.08731431014215</v>
+      </c>
+      <c r="F8" s="9">
+        <f>'Initial Buys'!N40</f>
+        <v>1069.29</v>
+      </c>
+      <c r="G8" s="32">
+        <f>'2017'!U8</f>
+        <v>45.010000000000005</v>
+      </c>
+      <c r="H8" s="24">
+        <v>0</v>
+      </c>
+      <c r="I8" s="21">
+        <v>0</v>
+      </c>
+      <c r="J8" s="24">
+        <v>0</v>
+      </c>
+      <c r="K8" s="21">
+        <v>0</v>
+      </c>
+      <c r="L8" s="24">
+        <v>0</v>
+      </c>
+      <c r="M8" s="21">
+        <v>0</v>
+      </c>
+      <c r="N8" s="24">
+        <v>0</v>
+      </c>
+      <c r="O8" s="21">
+        <v>0</v>
+      </c>
+      <c r="P8" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="21">
+        <v>0</v>
+      </c>
+      <c r="R8" s="24">
+        <v>0</v>
+      </c>
+      <c r="S8" s="21">
+        <v>0</v>
+      </c>
+      <c r="T8" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U8" s="17">
+        <f t="shared" si="3"/>
+        <v>45.010000000000005</v>
+      </c>
+      <c r="V8" s="15">
+        <f t="shared" si="1"/>
+        <v>1114.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="6">
+        <v>23.465</v>
+      </c>
+      <c r="E9" s="34">
+        <f t="shared" si="0"/>
+        <v>82.335393138717237</v>
+      </c>
+      <c r="F9" s="7">
+        <f>'Initial Buys'!Q40</f>
+        <v>1892.99</v>
+      </c>
+      <c r="G9" s="27">
+        <f>'2017'!U9</f>
+        <v>39.01</v>
+      </c>
+      <c r="H9" s="24">
+        <v>0</v>
+      </c>
+      <c r="I9" s="21">
+        <v>0</v>
+      </c>
+      <c r="J9" s="24">
+        <v>0</v>
+      </c>
+      <c r="K9" s="21">
+        <v>0</v>
+      </c>
+      <c r="L9" s="24">
+        <v>0</v>
+      </c>
+      <c r="M9" s="21">
+        <v>0</v>
+      </c>
+      <c r="N9" s="24">
+        <v>0</v>
+      </c>
+      <c r="O9" s="21">
+        <v>0</v>
+      </c>
+      <c r="P9" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="21">
+        <v>0</v>
+      </c>
+      <c r="R9" s="24">
+        <v>0</v>
+      </c>
+      <c r="S9" s="21">
+        <v>0</v>
+      </c>
+      <c r="T9" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U9" s="18">
+        <f t="shared" si="3"/>
+        <v>39.01</v>
+      </c>
+      <c r="V9" s="16">
+        <f t="shared" si="1"/>
+        <v>1932</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="8">
+        <v>8.3320000000000007</v>
+      </c>
+      <c r="E10" s="33">
+        <f t="shared" si="0"/>
+        <v>119.31108977436389</v>
+      </c>
+      <c r="F10" s="9">
+        <f>'Initial Buys'!T40</f>
+        <v>948</v>
+      </c>
+      <c r="G10" s="32">
+        <f>'2017'!U10</f>
+        <v>46.1</v>
+      </c>
+      <c r="H10" s="24">
+        <v>0</v>
+      </c>
+      <c r="I10" s="21">
+        <v>0</v>
+      </c>
+      <c r="J10" s="24">
+        <v>0</v>
+      </c>
+      <c r="K10" s="21">
+        <v>0</v>
+      </c>
+      <c r="L10" s="24">
+        <v>0</v>
+      </c>
+      <c r="M10" s="21">
+        <v>0</v>
+      </c>
+      <c r="N10" s="24">
+        <v>0</v>
+      </c>
+      <c r="O10" s="21">
+        <v>0</v>
+      </c>
+      <c r="P10" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="21">
+        <v>0</v>
+      </c>
+      <c r="R10" s="24">
+        <v>0</v>
+      </c>
+      <c r="S10" s="21">
+        <v>0</v>
+      </c>
+      <c r="T10" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U10" s="17">
+        <f t="shared" si="3"/>
+        <v>46.1</v>
+      </c>
+      <c r="V10" s="15">
+        <f t="shared" si="1"/>
+        <v>994.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="6">
+        <v>11.27</v>
+      </c>
+      <c r="E11" s="34">
+        <f t="shared" si="0"/>
+        <v>96.142857142857139</v>
+      </c>
+      <c r="F11" s="7">
+        <f>'Initial Buys'!W40</f>
+        <v>1062.5999999999999</v>
+      </c>
+      <c r="G11" s="27">
+        <f>'2017'!U11</f>
+        <v>20.93</v>
+      </c>
+      <c r="H11" s="24">
+        <v>0</v>
+      </c>
+      <c r="I11" s="21">
+        <v>0</v>
+      </c>
+      <c r="J11" s="24">
+        <v>0</v>
+      </c>
+      <c r="K11" s="21">
+        <v>0</v>
+      </c>
+      <c r="L11" s="24">
+        <v>0</v>
+      </c>
+      <c r="M11" s="21">
+        <v>0</v>
+      </c>
+      <c r="N11" s="24">
+        <v>0</v>
+      </c>
+      <c r="O11" s="21">
+        <v>0</v>
+      </c>
+      <c r="P11" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="21">
+        <v>0</v>
+      </c>
+      <c r="R11" s="24">
+        <v>0</v>
+      </c>
+      <c r="S11" s="21">
+        <v>0</v>
+      </c>
+      <c r="T11" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U11" s="18">
+        <f t="shared" si="3"/>
+        <v>20.93</v>
+      </c>
+      <c r="V11" s="16">
+        <f t="shared" si="1"/>
+        <v>1083.53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="8">
+        <v>4.0430000000000001</v>
+      </c>
+      <c r="E12" s="33">
+        <f t="shared" si="0"/>
+        <v>213.04724214692058</v>
+      </c>
+      <c r="F12" s="9">
+        <f>'Initial Buys'!L83</f>
+        <v>851.92</v>
+      </c>
+      <c r="G12" s="32">
+        <f>'2017'!U12</f>
+        <v>9.43</v>
+      </c>
+      <c r="H12" s="24">
+        <v>0</v>
+      </c>
+      <c r="I12" s="21">
+        <v>0</v>
+      </c>
+      <c r="J12" s="24">
+        <v>0</v>
+      </c>
+      <c r="K12" s="21">
+        <v>0</v>
+      </c>
+      <c r="L12" s="24">
+        <v>0</v>
+      </c>
+      <c r="M12" s="21">
+        <v>0</v>
+      </c>
+      <c r="N12" s="24">
+        <v>0</v>
+      </c>
+      <c r="O12" s="21">
+        <v>0</v>
+      </c>
+      <c r="P12" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="21">
+        <v>0</v>
+      </c>
+      <c r="R12" s="24">
+        <v>0</v>
+      </c>
+      <c r="S12" s="21">
+        <v>0</v>
+      </c>
+      <c r="T12" s="37">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U12" s="17">
+        <f t="shared" si="3"/>
+        <v>9.43</v>
+      </c>
+      <c r="V12" s="15">
+        <f t="shared" si="1"/>
+        <v>861.34999999999991</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="6">
+        <v>10.073</v>
+      </c>
+      <c r="E13" s="34">
+        <f t="shared" si="0"/>
+        <v>117.28055197061451</v>
+      </c>
+      <c r="F13" s="7">
+        <f>'Initial Buys'!O83</f>
+        <v>1173.317</v>
+      </c>
+      <c r="G13" s="27">
+        <f>'2017'!U13</f>
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="H13" s="24">
+        <v>0</v>
+      </c>
+      <c r="I13" s="21">
+        <v>0</v>
+      </c>
+      <c r="J13" s="24">
+        <v>0</v>
+      </c>
+      <c r="K13" s="21">
+        <v>0</v>
+      </c>
+      <c r="L13" s="24">
+        <v>0</v>
+      </c>
+      <c r="M13" s="21">
+        <v>0</v>
+      </c>
+      <c r="N13" s="24">
+        <v>0</v>
+      </c>
+      <c r="O13" s="21">
+        <v>0</v>
+      </c>
+      <c r="P13" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="21">
+        <v>0</v>
+      </c>
+      <c r="R13" s="24">
+        <v>0</v>
+      </c>
+      <c r="S13" s="21">
+        <v>0</v>
+      </c>
+      <c r="T13" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U13" s="18">
+        <f t="shared" si="3"/>
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="V13" s="16">
+        <f t="shared" si="1"/>
+        <v>1181.367</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="8">
+        <v>17.311</v>
+      </c>
+      <c r="E14" s="33">
+        <f t="shared" si="0"/>
+        <v>120.30327537403964</v>
+      </c>
+      <c r="F14" s="9">
+        <f>'Initial Buys'!Z40</f>
+        <v>2044.73</v>
+      </c>
+      <c r="G14" s="32">
+        <f>'2017'!U14</f>
+        <v>37.840000000000003</v>
+      </c>
+      <c r="H14" s="24">
+        <v>0</v>
+      </c>
+      <c r="I14" s="21">
+        <v>0</v>
+      </c>
+      <c r="J14" s="24">
+        <v>0</v>
+      </c>
+      <c r="K14" s="21">
+        <v>0</v>
+      </c>
+      <c r="L14" s="24">
+        <v>0</v>
+      </c>
+      <c r="M14" s="21">
+        <v>0</v>
+      </c>
+      <c r="N14" s="24">
+        <v>0</v>
+      </c>
+      <c r="O14" s="21">
+        <v>0</v>
+      </c>
+      <c r="P14" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="21">
+        <v>0</v>
+      </c>
+      <c r="R14" s="24">
+        <v>0</v>
+      </c>
+      <c r="S14" s="21">
+        <v>0</v>
+      </c>
+      <c r="T14" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U14" s="17">
+        <f t="shared" si="3"/>
+        <v>37.840000000000003</v>
+      </c>
+      <c r="V14" s="15">
+        <f t="shared" si="1"/>
+        <v>2082.5700000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="6">
+        <v>20.471</v>
+      </c>
+      <c r="E15" s="34">
+        <f t="shared" si="0"/>
+        <v>49.960431830394214</v>
+      </c>
+      <c r="F15" s="7">
+        <f>'Initial Buys'!I83</f>
+        <v>999.4</v>
+      </c>
+      <c r="G15" s="27">
+        <f>'2017'!U15</f>
+        <v>23.34</v>
+      </c>
+      <c r="H15" s="24">
+        <v>0</v>
+      </c>
+      <c r="I15" s="21">
+        <v>0</v>
+      </c>
+      <c r="J15" s="24">
+        <v>0</v>
+      </c>
+      <c r="K15" s="21">
+        <v>0</v>
+      </c>
+      <c r="L15" s="24">
+        <v>0</v>
+      </c>
+      <c r="M15" s="21">
+        <v>0</v>
+      </c>
+      <c r="N15" s="24">
+        <v>0</v>
+      </c>
+      <c r="O15" s="21">
+        <v>0</v>
+      </c>
+      <c r="P15" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="21">
+        <v>0</v>
+      </c>
+      <c r="R15" s="24">
+        <v>0</v>
+      </c>
+      <c r="S15" s="21">
+        <v>0</v>
+      </c>
+      <c r="T15" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U15" s="18">
+        <f t="shared" si="3"/>
+        <v>23.34</v>
+      </c>
+      <c r="V15" s="16">
+        <f t="shared" si="1"/>
+        <v>1022.74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="8">
+        <v>35.188000000000002</v>
+      </c>
+      <c r="E16" s="33">
+        <f>V16/D16</f>
+        <v>39.793679663521644</v>
+      </c>
+      <c r="F16" s="9">
+        <f>'Initial Buys'!AF40</f>
+        <v>1356.1799999999998</v>
+      </c>
+      <c r="G16" s="32">
+        <f>'2017'!U16</f>
+        <v>44.08</v>
+      </c>
+      <c r="H16" s="24">
+        <v>0</v>
+      </c>
+      <c r="I16" s="21">
+        <v>0</v>
+      </c>
+      <c r="J16" s="24">
+        <v>0</v>
+      </c>
+      <c r="K16" s="21">
+        <v>0</v>
+      </c>
+      <c r="L16" s="24">
+        <v>0</v>
+      </c>
+      <c r="M16" s="21">
+        <v>0</v>
+      </c>
+      <c r="N16" s="24">
+        <v>0</v>
+      </c>
+      <c r="O16" s="21">
+        <v>0</v>
+      </c>
+      <c r="P16" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="21">
+        <v>0</v>
+      </c>
+      <c r="R16" s="24">
+        <v>0</v>
+      </c>
+      <c r="S16" s="21">
+        <v>0</v>
+      </c>
+      <c r="T16" s="17">
+        <f>SUM(H16:S16)</f>
+        <v>0</v>
+      </c>
+      <c r="U16" s="17">
+        <f>SUM(G16:S16)</f>
+        <v>44.08</v>
+      </c>
+      <c r="V16" s="15">
+        <f>SUM(F16, U16)</f>
+        <v>1400.2599999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="6">
+        <v>15.603999999999999</v>
+      </c>
+      <c r="E17" s="34">
+        <f>V17/D17</f>
+        <v>72.101384260446054</v>
+      </c>
+      <c r="F17" s="7">
+        <f>'Initial Buys'!AC40</f>
+        <v>1078.6500000000001</v>
+      </c>
+      <c r="G17" s="27">
+        <f>'2017'!U17</f>
+        <v>38.5</v>
+      </c>
+      <c r="H17" s="24">
+        <v>7.92</v>
+      </c>
+      <c r="I17" s="21">
+        <v>0</v>
+      </c>
+      <c r="J17" s="24">
+        <v>0</v>
+      </c>
+      <c r="K17" s="21">
+        <v>0</v>
+      </c>
+      <c r="L17" s="24">
+        <v>0</v>
+      </c>
+      <c r="M17" s="21">
+        <v>0</v>
+      </c>
+      <c r="N17" s="24">
+        <v>0</v>
+      </c>
+      <c r="O17" s="21">
+        <v>0</v>
+      </c>
+      <c r="P17" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="21">
+        <v>0</v>
+      </c>
+      <c r="R17" s="24">
+        <v>0</v>
+      </c>
+      <c r="S17" s="21">
+        <v>0</v>
+      </c>
+      <c r="T17" s="18">
+        <f>SUM(H17:S17)</f>
+        <v>7.92</v>
+      </c>
+      <c r="U17" s="18">
+        <f>SUM(G17:S17)</f>
+        <v>46.42</v>
+      </c>
+      <c r="V17" s="16">
+        <f>SUM(F17, U17)</f>
+        <v>1125.0700000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="8">
+        <v>12.458</v>
+      </c>
+      <c r="E18" s="33">
+        <f t="shared" ref="E18" si="6">V18/D18</f>
+        <v>86.684058436346135</v>
+      </c>
+      <c r="F18" s="9">
+        <f>'Initial Buys'!B83</f>
+        <v>1042.68</v>
+      </c>
+      <c r="G18" s="32">
+        <f>'2017'!U18</f>
+        <v>37.230000000000004</v>
+      </c>
+      <c r="H18" s="24">
+        <v>0</v>
+      </c>
+      <c r="I18" s="21">
+        <v>0</v>
+      </c>
+      <c r="J18" s="24">
+        <v>0</v>
+      </c>
+      <c r="K18" s="21">
+        <v>0</v>
+      </c>
+      <c r="L18" s="24">
+        <v>0</v>
+      </c>
+      <c r="M18" s="21">
+        <v>0</v>
+      </c>
+      <c r="N18" s="24">
+        <v>0</v>
+      </c>
+      <c r="O18" s="21">
+        <v>0</v>
+      </c>
+      <c r="P18" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="21">
+        <v>0</v>
+      </c>
+      <c r="R18" s="24">
+        <v>0</v>
+      </c>
+      <c r="S18" s="21">
+        <v>0</v>
+      </c>
+      <c r="T18" s="17">
+        <f t="shared" ref="T18" si="7">SUM(H18:S18)</f>
+        <v>0</v>
+      </c>
+      <c r="U18" s="17">
+        <f t="shared" ref="U18" si="8">SUM(G18:S18)</f>
+        <v>37.230000000000004</v>
+      </c>
+      <c r="V18" s="15">
+        <f t="shared" ref="V18" si="9">SUM(F18, U18)</f>
+        <v>1079.9100000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="28"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="29">
+        <f t="shared" ref="F19:V19" si="10">SUM(F2:F18)</f>
+        <v>21416.587000000003</v>
+      </c>
+      <c r="G19" s="30">
+        <f t="shared" si="10"/>
+        <v>514.79000000000008</v>
+      </c>
+      <c r="H19" s="31">
+        <f t="shared" si="10"/>
+        <v>7.92</v>
+      </c>
+      <c r="I19" s="30">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="31">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="30">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L19" s="31">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="M19" s="30">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="31">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="30">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P19" s="31">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="30">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="R19" s="31">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="S19" s="30">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="T19" s="30">
+        <f t="shared" si="10"/>
+        <v>7.92</v>
+      </c>
+      <c r="U19" s="30">
+        <f t="shared" si="10"/>
+        <v>522.71</v>
+      </c>
+      <c r="V19" s="23">
+        <f t="shared" si="10"/>
+        <v>21939.297000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>